<commit_message>
more validations on clinic and person contact forms. cleaned up screening form to auto-calculate eligibility
</commit_message>
<xml_diff>
--- a/config/default/forms/app/contact_follow_up.xlsx
+++ b/config/default/forms/app/contact_follow_up.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="257">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -492,45 +492,27 @@
     <t xml:space="preserve">group_follow_up</t>
   </si>
   <si>
-    <t xml:space="preserve">Contact details</t>
+    <t xml:space="preserve">Tracing details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one select_follow_up_method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">follow_up_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How are you following up?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not(selected(.,'phone') and ${phone} = '')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There's no registered phone number</t>
   </si>
   <si>
     <t xml:space="preserve">note</t>
   </si>
   <si>
-    <t xml:space="preserve">n_details</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**Name:** ${name}  **Date of birth:** ${date_of_birth} **Phone number:** ${phone}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date_last_contact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**Date of last contact:** ${date_of_last_contact}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">floor(decimal-date-time(.)) &lt;= floor(decimal-date-time(today()))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date must not be in the future</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select_one select_follow_up_method</t>
-  </si>
-  <si>
-    <t xml:space="preserve">follow_up_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How are you following up?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">not(selected(.,'phone') and ${phone} = '')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There's no registered phone number</t>
-  </si>
-  <si>
     <t xml:space="preserve">call_button</t>
   </si>
   <si>
@@ -597,12 +579,6 @@
     <t xml:space="preserve">${status_call} = 'responded' or ${status_visit}= 'available'</t>
   </si>
   <si>
-    <t xml:space="preserve">health_care_worker_handed_to</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Health Care Worker handed to</t>
-  </si>
-  <si>
     <t xml:space="preserve">unique_patient_number</t>
   </si>
   <si>
@@ -717,7 +693,7 @@
     <t xml:space="preserve">responded</t>
   </si>
   <si>
-    <t xml:space="preserve">Contacted and linked</t>
+    <t xml:space="preserve">Contacted and already on ART</t>
   </si>
   <si>
     <t xml:space="preserve">responded_not_linked</t>
@@ -826,14 +802,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="167" formatCode="@"/>
-    <numFmt numFmtId="168" formatCode="MM/DD/YY"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -975,6 +950,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -1082,7 +1063,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1159,14 +1140,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1183,20 +1156,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1239,11 +1208,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="22" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="23" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1689,32 +1662,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AL92"/>
+  <dimension ref="A1:AL89"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B92" activeCellId="0" sqref="B92"/>
+      <selection pane="bottomLeft" activeCell="D79" activeCellId="0" sqref="D79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.6851063829787"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="33.6255319148936"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="55.6170212765957"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.0425531914894"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.7829787234043"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.0425531914894"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.2042553191489"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.0425531914894"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="48.7872340425532"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="42.5574468085106"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.0425531914894"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="74.4595744680851"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="27.5446808510638"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="23.0425531914894"/>
-    <col collapsed="false" hidden="false" max="38" min="15" style="0" width="11.0340425531915"/>
-    <col collapsed="false" hidden="false" max="1025" min="39" style="0" width="11.7829787234043"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.7148936170213"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="34.9787234042553"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="57.9446808510638"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.0170212765957"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.4340425531915"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.0170212765957"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.7829787234043"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.0170212765957"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="50.8170212765957"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="44.2851063829787"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="24.0170212765957"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="77.6127659574468"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="28.6723404255319"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="24.0170212765957"/>
+    <col collapsed="false" hidden="false" max="38" min="15" style="0" width="11.331914893617"/>
+    <col collapsed="false" hidden="false" max="1025" min="39" style="0" width="12.2340425531915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4721,7 +4694,7 @@
       </c>
       <c r="I70" s="13" t="str">
         <f aca="true">TEXT(NOW(), "yyyy-mm-dd")</f>
-        <v>2020-08-24</v>
+        <v>2020-08-25</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4758,599 +4731,518 @@
         <v>21</v>
       </c>
     </row>
-    <row r="73" s="20" customFormat="true" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="7" t="s">
+    <row r="73" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="B73" s="7" t="s">
+      <c r="B73" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="C73" s="7" t="s">
+      <c r="C73" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="D73" s="7" t="s">
+      <c r="D73" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="E73" s="19"/>
+      <c r="E73" s="21"/>
       <c r="F73" s="19"/>
-      <c r="G73" s="19"/>
-      <c r="H73" s="19"/>
-      <c r="I73" s="19"/>
-      <c r="J73" s="19"/>
+      <c r="G73" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="H73" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="I73" s="22"/>
+      <c r="J73" s="22"/>
       <c r="K73" s="19"/>
       <c r="L73" s="19"/>
-      <c r="M73" s="19"/>
+      <c r="M73" s="22"/>
       <c r="N73" s="19"/>
-    </row>
-    <row r="74" s="26" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="B74" s="22" t="s">
-        <v>159</v>
-      </c>
-      <c r="C74" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="D74" s="22" t="s">
+      <c r="P73" s="23"/>
+      <c r="Q73" s="23"/>
+      <c r="U73" s="23"/>
+    </row>
+    <row r="74" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="B74" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="C74" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="D74" s="20"/>
+      <c r="E74" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="F74" s="19"/>
+      <c r="G74" s="19"/>
+      <c r="H74" s="19"/>
+      <c r="I74" s="22"/>
+      <c r="J74" s="22"/>
+      <c r="K74" s="19"/>
+      <c r="L74" s="19"/>
+      <c r="M74" s="22"/>
+      <c r="N74" s="19"/>
+      <c r="P74" s="23"/>
+      <c r="Q74" s="23"/>
+      <c r="U74" s="23"/>
+    </row>
+    <row r="75" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="B75" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="C75" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="D75" s="20"/>
+      <c r="E75" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="F75" s="19"/>
+      <c r="G75" s="19"/>
+      <c r="H75" s="19"/>
+      <c r="I75" s="22"/>
+      <c r="J75" s="22"/>
+      <c r="K75" s="19"/>
+      <c r="L75" s="19"/>
+      <c r="M75" s="22"/>
+      <c r="N75" s="19"/>
+      <c r="P75" s="23"/>
+      <c r="Q75" s="23"/>
+      <c r="U75" s="23"/>
+    </row>
+    <row r="76" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="B76" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="C76" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="D76" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="E74" s="23"/>
-      <c r="F74" s="21"/>
-      <c r="G74" s="21" t="s">
+      <c r="E76" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="F76" s="19"/>
+      <c r="G76" s="19"/>
+      <c r="H76" s="19"/>
+      <c r="I76" s="19"/>
+      <c r="J76" s="19"/>
+      <c r="K76" s="19"/>
+      <c r="L76" s="22"/>
+      <c r="M76" s="22"/>
+      <c r="N76" s="19"/>
+      <c r="P76" s="23"/>
+      <c r="Q76" s="23"/>
+      <c r="U76" s="23"/>
+    </row>
+    <row r="77" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="B77" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="C77" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="D77" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E77" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="F77" s="19"/>
+      <c r="G77" s="19"/>
+      <c r="H77" s="19"/>
+      <c r="I77" s="19"/>
+      <c r="J77" s="19"/>
+      <c r="K77" s="19"/>
+      <c r="L77" s="22"/>
+      <c r="M77" s="22"/>
+      <c r="N77" s="19"/>
+      <c r="P77" s="23"/>
+      <c r="Q77" s="23"/>
+      <c r="U77" s="23"/>
+    </row>
+    <row r="78" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="B78" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="C78" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="D78" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E78" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="F78" s="19"/>
+      <c r="G78" s="19"/>
+      <c r="H78" s="19"/>
+      <c r="I78" s="19"/>
+      <c r="J78" s="19"/>
+      <c r="K78" s="19"/>
+      <c r="L78" s="22"/>
+      <c r="M78" s="22"/>
+      <c r="N78" s="19"/>
+      <c r="P78" s="23"/>
+      <c r="Q78" s="23"/>
+      <c r="U78" s="23"/>
+    </row>
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="B79" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="C79" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="D79" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E79" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="F79" s="19"/>
+      <c r="G79" s="19"/>
+      <c r="H79" s="19"/>
+      <c r="I79" s="19"/>
+      <c r="J79" s="19"/>
+      <c r="K79" s="19"/>
+      <c r="L79" s="22"/>
+      <c r="M79" s="22"/>
+      <c r="N79" s="19"/>
+      <c r="P79" s="23"/>
+      <c r="Q79" s="23"/>
+      <c r="U79" s="23"/>
+    </row>
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="B80" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="C80" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="D80" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E80" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="F80" s="19"/>
+      <c r="G80" s="19"/>
+      <c r="H80" s="19"/>
+      <c r="I80" s="19"/>
+      <c r="J80" s="19"/>
+      <c r="K80" s="22"/>
+      <c r="L80" s="22"/>
+      <c r="M80" s="22"/>
+      <c r="N80" s="19"/>
+      <c r="P80" s="23"/>
+      <c r="Q80" s="23"/>
+      <c r="U80" s="23"/>
+    </row>
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="B81" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="C81" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="D81" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E81" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="F81" s="19"/>
+      <c r="G81" s="19"/>
+      <c r="H81" s="19"/>
+      <c r="I81" s="19"/>
+      <c r="J81" s="19"/>
+      <c r="K81" s="22"/>
+      <c r="L81" s="22"/>
+      <c r="M81" s="22"/>
+      <c r="N81" s="19"/>
+      <c r="P81" s="23"/>
+      <c r="Q81" s="23"/>
+      <c r="U81" s="23"/>
+    </row>
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="H74" s="21" t="s">
-        <v>162</v>
-      </c>
-      <c r="I74" s="24"/>
-      <c r="J74" s="24"/>
-      <c r="K74" s="21"/>
-      <c r="L74" s="25" t="str">
-        <f aca="true">TEXT(NOW(), "yyyy-mm-dd")</f>
-        <v>2020-08-24</v>
-      </c>
-      <c r="M74" s="24"/>
-      <c r="N74" s="21"/>
-      <c r="P74" s="27"/>
-      <c r="Q74" s="27"/>
-      <c r="U74" s="27"/>
-    </row>
-    <row r="75" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="21" t="s">
-        <v>163</v>
-      </c>
-      <c r="B75" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="C75" s="22" t="s">
-        <v>165</v>
-      </c>
-      <c r="D75" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="E75" s="23"/>
-      <c r="F75" s="21"/>
-      <c r="G75" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="H75" s="21" t="s">
-        <v>167</v>
-      </c>
-      <c r="I75" s="24"/>
-      <c r="J75" s="24"/>
-      <c r="K75" s="21"/>
-      <c r="L75" s="21"/>
-      <c r="M75" s="24"/>
-      <c r="N75" s="21"/>
-      <c r="P75" s="27"/>
-      <c r="Q75" s="27"/>
-      <c r="U75" s="27"/>
-    </row>
-    <row r="76" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="B76" s="22" t="s">
-        <v>168</v>
-      </c>
-      <c r="C76" s="22" t="s">
-        <v>169</v>
-      </c>
-      <c r="D76" s="22"/>
-      <c r="E76" s="28" t="s">
-        <v>170</v>
-      </c>
-      <c r="F76" s="21"/>
-      <c r="G76" s="21"/>
-      <c r="H76" s="21"/>
-      <c r="I76" s="24"/>
-      <c r="J76" s="24"/>
-      <c r="K76" s="21"/>
-      <c r="L76" s="21"/>
-      <c r="M76" s="24"/>
-      <c r="N76" s="21"/>
-      <c r="P76" s="27"/>
-      <c r="Q76" s="27"/>
-      <c r="U76" s="27"/>
-    </row>
-    <row r="77" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="B77" s="22" t="s">
+      <c r="B82" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="27"/>
+      <c r="G82" s="28"/>
+      <c r="H82" s="28"/>
+      <c r="I82" s="28"/>
+      <c r="J82" s="28"/>
+      <c r="K82" s="28"/>
+      <c r="L82" s="28"/>
+      <c r="M82" s="28"/>
+      <c r="N82" s="28"/>
+    </row>
+    <row r="83" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="C77" s="22" t="s">
-        <v>172</v>
-      </c>
-      <c r="D77" s="22"/>
-      <c r="E77" s="28" t="s">
-        <v>173</v>
-      </c>
-      <c r="F77" s="21"/>
-      <c r="G77" s="21"/>
-      <c r="H77" s="21"/>
-      <c r="I77" s="24"/>
-      <c r="J77" s="24"/>
-      <c r="K77" s="21"/>
-      <c r="L77" s="21"/>
-      <c r="M77" s="24"/>
-      <c r="N77" s="21"/>
-      <c r="P77" s="27"/>
-      <c r="Q77" s="27"/>
-      <c r="U77" s="27"/>
-    </row>
-    <row r="78" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="21" t="s">
-        <v>174</v>
-      </c>
-      <c r="B78" s="22" t="s">
-        <v>175</v>
-      </c>
-      <c r="C78" s="22" t="s">
-        <v>176</v>
-      </c>
-      <c r="D78" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="E78" s="28" t="s">
-        <v>170</v>
-      </c>
-      <c r="F78" s="21"/>
-      <c r="G78" s="21"/>
-      <c r="H78" s="21"/>
-      <c r="I78" s="21"/>
-      <c r="J78" s="21"/>
-      <c r="K78" s="21"/>
-      <c r="L78" s="24"/>
-      <c r="M78" s="24"/>
-      <c r="N78" s="21"/>
-      <c r="P78" s="27"/>
-      <c r="Q78" s="27"/>
-      <c r="U78" s="27"/>
-    </row>
-    <row r="79" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="B79" s="22" t="s">
-        <v>178</v>
-      </c>
-      <c r="C79" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="D79" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="E79" s="28" t="s">
-        <v>180</v>
-      </c>
-      <c r="F79" s="21"/>
-      <c r="G79" s="21"/>
-      <c r="H79" s="21"/>
-      <c r="I79" s="21"/>
-      <c r="J79" s="21"/>
-      <c r="K79" s="21"/>
-      <c r="L79" s="24"/>
-      <c r="M79" s="24"/>
-      <c r="N79" s="21"/>
-      <c r="P79" s="27"/>
-      <c r="Q79" s="27"/>
-      <c r="U79" s="27"/>
-    </row>
-    <row r="80" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="21" t="s">
-        <v>181</v>
-      </c>
-      <c r="B80" s="22" t="s">
-        <v>182</v>
-      </c>
-      <c r="C80" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="D80" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="E80" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="F80" s="21"/>
-      <c r="G80" s="21"/>
-      <c r="H80" s="21"/>
-      <c r="I80" s="21"/>
-      <c r="J80" s="21"/>
-      <c r="K80" s="21"/>
-      <c r="L80" s="24"/>
-      <c r="M80" s="24"/>
-      <c r="N80" s="21"/>
-      <c r="P80" s="27"/>
-      <c r="Q80" s="27"/>
-      <c r="U80" s="27"/>
-    </row>
-    <row r="81" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="B81" s="22" t="s">
-        <v>185</v>
-      </c>
-      <c r="C81" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="D81" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="E81" s="26" t="s">
-        <v>186</v>
-      </c>
-      <c r="F81" s="21"/>
-      <c r="G81" s="21"/>
-      <c r="H81" s="21"/>
-      <c r="I81" s="21"/>
-      <c r="J81" s="21"/>
-      <c r="K81" s="21"/>
-      <c r="L81" s="24"/>
-      <c r="M81" s="24"/>
-      <c r="N81" s="21"/>
-      <c r="P81" s="27"/>
-      <c r="Q81" s="27"/>
-      <c r="U81" s="27"/>
-    </row>
-    <row r="82" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="B82" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="C82" s="22" t="s">
+      <c r="B83" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="D82" s="22"/>
-      <c r="E82" s="28" t="s">
+      <c r="C83" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="F82" s="21"/>
-      <c r="G82" s="21"/>
-      <c r="H82" s="21"/>
-      <c r="I82" s="21"/>
-      <c r="J82" s="21"/>
-      <c r="K82" s="24"/>
-      <c r="L82" s="24"/>
-      <c r="M82" s="24"/>
-      <c r="N82" s="21"/>
-      <c r="P82" s="27"/>
-      <c r="Q82" s="27"/>
-      <c r="U82" s="27"/>
-    </row>
-    <row r="83" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="B83" s="22" t="s">
+      <c r="D83" s="20"/>
+      <c r="E83" s="24"/>
+      <c r="F83" s="19"/>
+      <c r="G83" s="19"/>
+      <c r="H83" s="19"/>
+      <c r="I83" s="19"/>
+      <c r="J83" s="19"/>
+      <c r="K83" s="22"/>
+      <c r="L83" s="22"/>
+      <c r="M83" s="22"/>
+      <c r="N83" s="19"/>
+      <c r="P83" s="23"/>
+      <c r="Q83" s="23"/>
+      <c r="U83" s="23"/>
+    </row>
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B84" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="C83" s="22" t="s">
+      <c r="C84" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="D83" s="22"/>
-      <c r="E83" s="28" t="s">
-        <v>189</v>
-      </c>
-      <c r="F83" s="21"/>
-      <c r="G83" s="21"/>
-      <c r="H83" s="21"/>
-      <c r="I83" s="21"/>
-      <c r="J83" s="21"/>
-      <c r="K83" s="24"/>
-      <c r="L83" s="24"/>
-      <c r="M83" s="24"/>
-      <c r="N83" s="21"/>
-      <c r="P83" s="27"/>
-      <c r="Q83" s="27"/>
-      <c r="U83" s="27"/>
-    </row>
-    <row r="84" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="B84" s="22" t="s">
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="6"/>
+      <c r="J84" s="6"/>
+      <c r="K84" s="6"/>
+      <c r="L84" s="6"/>
+      <c r="M84" s="6"/>
+      <c r="N84" s="6"/>
+    </row>
+    <row r="85" s="25" customFormat="true" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B85" s="20" t="s">
         <v>192</v>
       </c>
-      <c r="C84" s="22" t="s">
+      <c r="C85" s="20"/>
+      <c r="D85" s="19"/>
+      <c r="E85" s="21"/>
+      <c r="F85" s="19"/>
+      <c r="G85" s="19"/>
+      <c r="H85" s="19"/>
+      <c r="I85" s="22"/>
+      <c r="J85" s="19"/>
+      <c r="K85" s="19"/>
+      <c r="L85" s="22"/>
+      <c r="M85" s="22"/>
+      <c r="N85" s="19"/>
+      <c r="P85" s="23"/>
+      <c r="Q85" s="23"/>
+      <c r="U85" s="23"/>
+    </row>
+    <row r="86" s="18" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A87" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B87" s="29" t="s">
         <v>193</v>
       </c>
-      <c r="D84" s="22"/>
-      <c r="E84" s="28" t="s">
-        <v>189</v>
-      </c>
-      <c r="F84" s="21"/>
-      <c r="G84" s="21"/>
-      <c r="H84" s="21"/>
-      <c r="I84" s="21"/>
-      <c r="J84" s="21"/>
-      <c r="K84" s="24"/>
-      <c r="L84" s="24"/>
-      <c r="M84" s="24"/>
-      <c r="N84" s="21"/>
-      <c r="P84" s="27"/>
-      <c r="Q84" s="27"/>
-      <c r="U84" s="27"/>
-    </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="29" t="s">
-        <v>156</v>
-      </c>
-      <c r="B85" s="6" t="s">
+      <c r="C87" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D87" s="27"/>
+      <c r="E87" s="27"/>
+      <c r="F87" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="G87" s="27"/>
+      <c r="H87" s="27"/>
+      <c r="I87" s="27"/>
+      <c r="J87" s="27"/>
+      <c r="K87" s="27"/>
+      <c r="L87" s="27"/>
+      <c r="M87" s="27"/>
+      <c r="N87" s="27"/>
+    </row>
+    <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A88" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B88" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="C85" s="6" t="s">
+      <c r="C88" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D88" s="28"/>
+      <c r="E88" s="31"/>
+      <c r="F88" s="31"/>
+      <c r="G88" s="31"/>
+      <c r="H88" s="31"/>
+      <c r="I88" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="D85" s="6"/>
-      <c r="E85" s="6"/>
-      <c r="F85" s="30"/>
-      <c r="G85" s="31"/>
-      <c r="H85" s="31"/>
-      <c r="I85" s="31"/>
-      <c r="J85" s="31"/>
-      <c r="K85" s="31"/>
-      <c r="L85" s="31"/>
-      <c r="M85" s="31"/>
-      <c r="N85" s="31"/>
-    </row>
-    <row r="86" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="B86" s="22" t="s">
-        <v>196</v>
-      </c>
-      <c r="C86" s="22" t="s">
-        <v>197</v>
-      </c>
-      <c r="D86" s="22"/>
-      <c r="E86" s="28"/>
-      <c r="F86" s="21"/>
-      <c r="G86" s="21"/>
-      <c r="H86" s="21"/>
-      <c r="I86" s="21"/>
-      <c r="J86" s="21"/>
-      <c r="K86" s="24"/>
-      <c r="L86" s="24"/>
-      <c r="M86" s="24"/>
-      <c r="N86" s="21"/>
-      <c r="P86" s="27"/>
-      <c r="Q86" s="27"/>
-      <c r="U86" s="27"/>
-    </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="B87" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="C87" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="D87" s="6"/>
-      <c r="E87" s="6"/>
-      <c r="F87" s="6"/>
-      <c r="G87" s="6"/>
-      <c r="H87" s="6"/>
-      <c r="I87" s="6"/>
-      <c r="J87" s="6"/>
-      <c r="K87" s="6"/>
-      <c r="L87" s="6"/>
-      <c r="M87" s="6"/>
-      <c r="N87" s="6"/>
-    </row>
-    <row r="88" s="26" customFormat="true" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B88" s="22" t="s">
-        <v>200</v>
-      </c>
-      <c r="C88" s="22"/>
-      <c r="D88" s="21"/>
-      <c r="E88" s="23"/>
-      <c r="F88" s="21"/>
-      <c r="G88" s="21"/>
-      <c r="H88" s="21"/>
-      <c r="I88" s="24"/>
-      <c r="J88" s="21"/>
-      <c r="K88" s="21"/>
-      <c r="L88" s="24"/>
-      <c r="M88" s="24"/>
-      <c r="N88" s="21"/>
-      <c r="P88" s="27"/>
-      <c r="Q88" s="27"/>
-      <c r="U88" s="27"/>
-    </row>
-    <row r="89" s="18" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="18" t="s">
+      <c r="J88" s="31"/>
+      <c r="K88" s="31"/>
+      <c r="L88" s="31"/>
+      <c r="M88" s="31"/>
+      <c r="N88" s="31"/>
+    </row>
+    <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A89" s="32" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A90" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="B90" s="32" t="s">
-        <v>201</v>
-      </c>
-      <c r="C90" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="D90" s="30"/>
-      <c r="E90" s="30"/>
-      <c r="F90" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="G90" s="30"/>
-      <c r="H90" s="30"/>
-      <c r="I90" s="30"/>
-      <c r="J90" s="30"/>
-      <c r="K90" s="30"/>
-      <c r="L90" s="30"/>
-      <c r="M90" s="30"/>
-      <c r="N90" s="30"/>
-    </row>
-    <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="B91" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="C91" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D91" s="31"/>
-      <c r="E91" s="34"/>
-      <c r="F91" s="34"/>
-      <c r="G91" s="34"/>
-      <c r="H91" s="34"/>
-      <c r="I91" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="J91" s="34"/>
-      <c r="K91" s="34"/>
-      <c r="L91" s="34"/>
-      <c r="M91" s="34"/>
-      <c r="N91" s="34"/>
-    </row>
-    <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="B92" s="30"/>
-      <c r="C92" s="30"/>
-      <c r="D92" s="30"/>
-      <c r="E92" s="30"/>
-      <c r="F92" s="30"/>
-      <c r="G92" s="30"/>
-      <c r="H92" s="30"/>
-      <c r="I92" s="30"/>
-      <c r="J92" s="30"/>
-      <c r="K92" s="30"/>
-      <c r="L92" s="30"/>
-      <c r="M92" s="30"/>
-      <c r="N92" s="30"/>
+      <c r="B89" s="27"/>
+      <c r="C89" s="27"/>
+      <c r="D89" s="27"/>
+      <c r="E89" s="27"/>
+      <c r="F89" s="27"/>
+      <c r="G89" s="27"/>
+      <c r="H89" s="27"/>
+      <c r="I89" s="27"/>
+      <c r="J89" s="27"/>
+      <c r="K89" s="27"/>
+      <c r="L89" s="27"/>
+      <c r="M89" s="27"/>
+      <c r="N89" s="27"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A85">
+  <conditionalFormatting sqref="A82">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E85">
+  <conditionalFormatting sqref="E82">
     <cfRule type="containsText" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E85">
+  <conditionalFormatting sqref="E82">
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>AND($A85="begin group", NOT($B85 = ""))</formula>
+      <formula>AND($A82="begin group", NOT($B82 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E85">
+  <conditionalFormatting sqref="E82">
     <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
-      <formula>AND($A85="end group", $B85 = "", $C85 = "", $D85 = "", $E85 = "", $F85 = "", $G85 = "", $H85 = "", $I85 = "", $J85 = "", $K85 = "", $L85 = "", $M85 = "")</formula>
+      <formula>AND($A82="end group", $B82 = "", $C82 = "", $D82 = "", $E82 = "", $F82 = "", $G82 = "", $H82 = "", $I82 = "", $J82 = "", $K82 = "", $L82 = "", $M82 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E85">
+  <conditionalFormatting sqref="E82">
     <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E85">
+  <conditionalFormatting sqref="E82">
     <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
-      <formula>AND($A85="begin repeat", NOT($B85 = ""))</formula>
+      <formula>AND($A82="begin repeat", NOT($B82 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E85">
+  <conditionalFormatting sqref="E82">
     <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
-      <formula>AND($A85="end repeat", $B85 = "", $C85 = "", $D85 = "", $E85 = "", $F85 = "", $G85 = "", $H85 = "", $I85 = "", $J85 = "", $K85 = "", $L85 = "", $M85 = "")</formula>
+      <formula>AND($A82="end repeat", $B82 = "", $C82 = "", $D82 = "", $E82 = "", $F82 = "", $G82 = "", $H82 = "", $I82 = "", $J82 = "", $K82 = "", $L82 = "", $M82 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E87">
+  <conditionalFormatting sqref="E84">
     <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
-      <formula>AND($A87="begin group", NOT($B87 = ""))</formula>
+      <formula>AND($A84="begin group", NOT($B84 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E87">
+  <conditionalFormatting sqref="E84">
     <cfRule type="cellIs" priority="10" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I87">
+  <conditionalFormatting sqref="I84">
     <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
-      <formula>AND($I87 = "", $A87 = "calculate")</formula>
+      <formula>AND($I84 = "", $A84 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C87">
+  <conditionalFormatting sqref="C84">
     <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
-      <formula>AND(AND(NOT($A87 = "end group"), NOT($A87 = "end repeat"), NOT($A87 = "")), $C87 = "")</formula>
+      <formula>AND(AND(NOT($A84 = "end group"), NOT($A84 = "end repeat"), NOT($A84 = "")), $C84 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B87">
+  <conditionalFormatting sqref="B84">
     <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
-      <formula>AND(AND(NOT($A87 = "end group"), NOT($A87 = "end repeat"), NOT($A87 = "")), $B87 = "")</formula>
+      <formula>AND(AND(NOT($A84 = "end group"), NOT($A84 = "end repeat"), NOT($A84 = "")), $B84 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A87">
+  <conditionalFormatting sqref="A84">
     <cfRule type="cellIs" priority="14" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H87">
+  <conditionalFormatting sqref="H84">
     <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
-      <formula>AND(NOT($G87 = ""), $H87 = "")</formula>
+      <formula>AND(NOT($G84 = ""), $H84 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E87">
+  <conditionalFormatting sqref="E84">
     <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
-      <formula>AND($A87="begin repeat", NOT($B87 = ""))</formula>
+      <formula>AND($A84="begin repeat", NOT($B84 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E87">
+  <conditionalFormatting sqref="E84">
     <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
-      <formula>AND($E87 = "", $A87 = "calculate")</formula>
+      <formula>AND($E84 = "", $A84 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E87">
+  <conditionalFormatting sqref="E84">
     <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
-      <formula>AND($A87="end repeat", $B87 = "", $C87 = "", $D87 = "", $E87 = "", $F87 = "", $G87 = "", $H87 = "", $E87 = "", $J87 = "", $K87 = "", $L87 = "", $M87 = "")</formula>
+      <formula>AND($A84="end repeat", $B84 = "", $C84 = "", $D84 = "", $E84 = "", $F84 = "", $G84 = "", $H84 = "", $E84 = "", $J84 = "", $K84 = "", $L84 = "", $M84 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E87">
+  <conditionalFormatting sqref="E84">
     <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
-      <formula>AND($A87="end group", $B87 = "", $C87 = "", $D87 = "", $E87 = "", $F87 = "", $G87 = "", $H87 = "", $E87 = "", $J87 = "", $K87 = "", $L87 = "", $M87 = "")</formula>
+      <formula>AND($A84="end group", $B84 = "", $C84 = "", $D84 = "", $E84 = "", $F84 = "", $G84 = "", $H84 = "", $E84 = "", $J84 = "", $K84 = "", $L84 = "", $M84 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E87">
+  <conditionalFormatting sqref="E84">
     <cfRule type="containsText" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:Y13">
@@ -5395,7 +5287,7 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
     <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27">
-      <formula>COUNTIF($B$2:$B$1055,B13)&gt;1</formula>
+      <formula>COUNTIF($B$2:$B$1052,B13)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:Y13">
@@ -5412,11 +5304,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D11:D13 D85 D87" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D11:D13 D82 D84" type="list">
       <formula1>"yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D3:D7 D90:D92" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D3:D7 D87:D89" type="list">
       <formula1>"yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5438,512 +5330,512 @@
   </sheetPr>
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="35.8042553191489"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="11.0340425531915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="29.8723404255319"/>
-    <col collapsed="false" hidden="false" max="26" min="4" style="0" width="11.0340425531915"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="11.7829787234043"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="37.2297872340426"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="11.331914893617"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="31.0765957446808"/>
+    <col collapsed="false" hidden="false" max="26" min="4" style="0" width="11.331914893617"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="12.2340425531915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="33" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="34" t="s">
+        <v>198</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="34" t="s">
+        <v>198</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="C4" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="36" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="B6" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="36" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="37" t="s">
-        <v>206</v>
-      </c>
-      <c r="B2" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="37" t="s">
+      <c r="C6" s="20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="20" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="37" t="s">
-        <v>206</v>
-      </c>
-      <c r="B3" s="37" t="s">
+      <c r="B7" s="20" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="20" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="B8" s="20" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" s="20" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="B9" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="C9" s="20" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="B10" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="C10" s="20" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="B11" s="20" t="n">
+        <v>6</v>
+      </c>
+      <c r="C11" s="20" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="B12" s="20" t="n">
+        <v>7</v>
+      </c>
+      <c r="C12" s="20" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="B13" s="20" t="n">
+        <v>8</v>
+      </c>
+      <c r="C13" s="20" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="B14" s="20" t="n">
+        <v>9</v>
+      </c>
+      <c r="C14" s="20" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="B15" s="20" t="n">
+        <v>10</v>
+      </c>
+      <c r="C15" s="20" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="B16" s="20" t="n">
+        <v>11</v>
+      </c>
+      <c r="C16" s="20" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="B17" s="20" t="n">
+        <v>12</v>
+      </c>
+      <c r="C17" s="20" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="B18" s="20" t="n">
+        <v>13</v>
+      </c>
+      <c r="C18" s="20" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="B19" s="20" t="n">
+        <v>14</v>
+      </c>
+      <c r="C19" s="20" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="B20" s="20" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22" t="s">
+      <c r="C20" s="20" t="s">
         <v>210</v>
       </c>
-      <c r="B4" s="22" t="s">
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="20" t="s">
         <v>211</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="B22" s="20" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22" t="s">
-        <v>210</v>
-      </c>
-      <c r="B5" s="22" t="s">
+      <c r="C22" s="20" t="s">
         <v>213</v>
       </c>
-      <c r="C5" s="22" t="s">
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="B23" s="20" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="22" t="s">
+      <c r="C23" s="20" t="s">
         <v>215</v>
       </c>
-      <c r="B6" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" s="22" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="B7" s="22" t="n">
-        <v>2</v>
-      </c>
-      <c r="C7" s="22" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="B8" s="22" t="n">
-        <v>3</v>
-      </c>
-      <c r="C8" s="22" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="B9" s="22" t="n">
-        <v>4</v>
-      </c>
-      <c r="C9" s="22" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="B10" s="22" t="n">
-        <v>5</v>
-      </c>
-      <c r="C10" s="22" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="B11" s="22" t="n">
-        <v>6</v>
-      </c>
-      <c r="C11" s="22" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="B12" s="22" t="n">
-        <v>7</v>
-      </c>
-      <c r="C12" s="22" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="B13" s="22" t="n">
-        <v>8</v>
-      </c>
-      <c r="C13" s="22" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="B14" s="22" t="n">
-        <v>9</v>
-      </c>
-      <c r="C14" s="22" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="B15" s="22" t="n">
-        <v>10</v>
-      </c>
-      <c r="C15" s="22" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="B16" s="22" t="n">
-        <v>11</v>
-      </c>
-      <c r="C16" s="22" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="B17" s="22" t="n">
-        <v>12</v>
-      </c>
-      <c r="C17" s="22" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="B18" s="22" t="n">
-        <v>13</v>
-      </c>
-      <c r="C18" s="22" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="B19" s="22" t="n">
-        <v>14</v>
-      </c>
-      <c r="C19" s="22" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="22" t="s">
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="B24" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="C24" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="C20" s="22" t="s">
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="B26" s="20" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="22" t="s">
-        <v>216</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="22" t="s">
+      <c r="C26" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="B22" s="22" t="s">
+    </row>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="20" t="s">
         <v>220</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="B27" s="20" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="22" t="s">
+      <c r="C27" s="35" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="B29" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="C29" s="36" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="C33" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="B23" s="22" t="s">
+    </row>
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>241</v>
+      </c>
+      <c r="C38" s="20" t="s">
         <v>222</v>
       </c>
-      <c r="C23" s="22" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="22" t="s">
+    </row>
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="B39" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="B42" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="C45" s="20" t="s">
         <v>219</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>224</v>
-      </c>
-      <c r="C24" s="22" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="22" t="s">
-        <v>219</v>
-      </c>
-      <c r="B25" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="C25" s="22" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="22" t="s">
-        <v>219</v>
-      </c>
-      <c r="B26" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="B27" s="22" t="s">
-        <v>229</v>
-      </c>
-      <c r="C27" s="22" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="B28" s="22" t="s">
-        <v>231</v>
-      </c>
-      <c r="C28" s="22" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="B29" s="22" t="s">
-        <v>233</v>
-      </c>
-      <c r="C29" s="38" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="B30" s="22" t="s">
-        <v>235</v>
-      </c>
-      <c r="C30" s="22" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="B31" s="22" t="s">
-        <v>237</v>
-      </c>
-      <c r="C31" s="22" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="B32" s="22" t="s">
-        <v>239</v>
-      </c>
-      <c r="C32" s="22" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="B33" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="C33" s="22" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="22" t="s">
-        <v>241</v>
-      </c>
-      <c r="B34" s="22" t="s">
-        <v>242</v>
-      </c>
-      <c r="C34" s="22" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="22" t="s">
-        <v>241</v>
-      </c>
-      <c r="B35" s="22" t="s">
-        <v>244</v>
-      </c>
-      <c r="C35" s="22" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="22" t="s">
-        <v>241</v>
-      </c>
-      <c r="B36" s="22" t="s">
-        <v>246</v>
-      </c>
-      <c r="C36" s="22" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="22" t="s">
-        <v>241</v>
-      </c>
-      <c r="B37" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="C37" s="22" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="22" t="s">
-        <v>248</v>
-      </c>
-      <c r="B38" s="22" t="s">
-        <v>249</v>
-      </c>
-      <c r="C38" s="22" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="22" t="s">
-        <v>248</v>
-      </c>
-      <c r="B39" s="22" t="s">
-        <v>250</v>
-      </c>
-      <c r="C39" s="22" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="22" t="s">
-        <v>248</v>
-      </c>
-      <c r="B40" s="22" t="s">
-        <v>222</v>
-      </c>
-      <c r="C40" s="22" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="22" t="s">
-        <v>248</v>
-      </c>
-      <c r="B41" s="22" t="s">
-        <v>252</v>
-      </c>
-      <c r="C41" s="22" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="22" t="s">
-        <v>248</v>
-      </c>
-      <c r="B42" s="22" t="s">
-        <v>254</v>
-      </c>
-      <c r="C42" s="22" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="22" t="s">
-        <v>248</v>
-      </c>
-      <c r="B43" s="22" t="s">
-        <v>255</v>
-      </c>
-      <c r="C43" s="22" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="22" t="s">
-        <v>248</v>
-      </c>
-      <c r="B44" s="22" t="s">
-        <v>239</v>
-      </c>
-      <c r="C44" s="22" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="22" t="s">
-        <v>248</v>
-      </c>
-      <c r="B45" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="C45" s="22" t="s">
-        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -5970,89 +5862,89 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1702127659574"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3957446808511"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.8808510638298"/>
-    <col collapsed="false" hidden="false" max="26" min="4" style="0" width="11.0340425531915"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="11.7829787234043"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1446808510638"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3702127659574"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.4553191489362"/>
+    <col collapsed="false" hidden="false" max="26" min="4" style="0" width="11.331914893617"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="12.2340425531915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="39" t="s">
-        <v>256</v>
-      </c>
-      <c r="B1" s="39" t="s">
-        <v>257</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>258</v>
-      </c>
-      <c r="D1" s="39" t="s">
-        <v>259</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>260</v>
-      </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
-      <c r="S1" s="40"/>
-      <c r="T1" s="40"/>
-      <c r="U1" s="40"/>
-      <c r="V1" s="40"/>
-      <c r="W1" s="40"/>
-      <c r="X1" s="40"/>
-      <c r="Y1" s="40"/>
-      <c r="Z1" s="40"/>
+      <c r="A1" s="37" t="s">
+        <v>248</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>249</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>250</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>252</v>
+      </c>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
     </row>
     <row r="2" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="41" t="s">
-        <v>261</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>262</v>
+      <c r="A2" s="39" t="s">
+        <v>253</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>254</v>
       </c>
       <c r="C2" s="1" t="str">
         <f aca="true">TEXT(NOW(), "yyyy-mm-dd")</f>
-        <v>2020-08-24</v>
-      </c>
-      <c r="D2" s="41" t="s">
-        <v>263</v>
-      </c>
-      <c r="E2" s="41" t="s">
-        <v>264</v>
-      </c>
-      <c r="F2" s="41"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="42"/>
-      <c r="P2" s="42"/>
-      <c r="Q2" s="42"/>
-      <c r="R2" s="42"/>
-      <c r="S2" s="42"/>
-      <c r="T2" s="42"/>
-      <c r="U2" s="42"/>
-      <c r="V2" s="42"/>
-      <c r="W2" s="42"/>
-      <c r="X2" s="42"/>
-      <c r="Y2" s="42"/>
-      <c r="Z2" s="42"/>
+        <v>2020-08-25</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>255</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>256</v>
+      </c>
+      <c r="F2" s="39"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="40"/>
+      <c r="W2" s="40"/>
+      <c r="X2" s="40"/>
+      <c r="Y2" s="40"/>
+      <c r="Z2" s="40"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
correctly show contact name for submitted contact followup reports
</commit_message>
<xml_diff>
--- a/config/default/forms/app/contact_follow_up.xlsx
+++ b/config/default/forms/app/contact_follow_up.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="229">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -198,48 +198,6 @@
     <t xml:space="preserve">Type of contact</t>
   </si>
   <si>
-    <t xml:space="preserve">case_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Case ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">case_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Case Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type_of_contact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Close Contact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">relation_to_case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relation to Case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">national_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">National ID Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">passport_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Passport Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alien_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alien Number</t>
-  </si>
-  <si>
     <t xml:space="preserve">s_name</t>
   </si>
   <si>
@@ -283,60 +241,6 @@
   </si>
   <si>
     <t xml:space="preserve">Marital Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">head_of_household</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Head of household</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date_of_last_contact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Occupation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">occupation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date of last contact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">occupation_other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other (specify)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">health_care_worker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is the contact a health care worker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">facility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If contact is health worker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">education</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Education</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deceased</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deceased</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date_of_death</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date of death</t>
   </si>
   <si>
     <t xml:space="preserve">nationality</t>
@@ -612,7 +516,13 @@
     <t xml:space="preserve">created_by</t>
   </si>
   <si>
-    <t xml:space="preserve">../../inputs/user/username</t>
+    <t xml:space="preserve">../inputs/user/username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patient_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../inputs/contact/name</t>
   </si>
   <si>
     <t xml:space="preserve">list_name</t>
@@ -679,6 +589,12 @@
   </si>
   <si>
     <t xml:space="preserve">Person not found in their usual place of residence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deceased</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deceased</t>
   </si>
   <si>
     <t xml:space="preserve">other</t>
@@ -808,7 +724,7 @@
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -950,12 +866,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -1063,7 +973,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1208,15 +1118,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="23" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="22" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1662,32 +1568,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AL89"/>
+  <dimension ref="A1:AL74"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D79" activeCellId="0" sqref="D79"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="I72" activeCellId="0" sqref="I72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.7148936170213"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="34.9787234042553"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="57.9446808510638"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.0170212765957"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.4340425531915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.0170212765957"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.7829787234043"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.0170212765957"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="50.8170212765957"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="44.2851063829787"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="24.0170212765957"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="77.6127659574468"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="28.6723404255319"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="24.0170212765957"/>
-    <col collapsed="false" hidden="false" max="38" min="15" style="0" width="11.331914893617"/>
-    <col collapsed="false" hidden="false" max="1025" min="39" style="0" width="12.2340425531915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.6893617021277"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="35.7276595744681"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="59.1446808510638"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.468085106383"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="42.331914893617"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.468085106383"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.6085106382979"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.468085106383"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="51.9404255319149"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="45.2595744680851"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="24.468085106383"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="79.2638297872341"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="29.2723404255319"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="24.468085106383"/>
+    <col collapsed="false" hidden="false" max="38" min="15" style="0" width="11.4851063829787"/>
+    <col collapsed="false" hidden="false" max="1025" min="39" style="0" width="12.4595744680851"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2370,7 +2276,7 @@
       <c r="A19" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="11" t="s">
         <v>58</v>
       </c>
       <c r="C19" s="10" t="s">
@@ -2378,9 +2284,7 @@
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
-      <c r="F19" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
@@ -2511,10 +2415,10 @@
         <v>29</v>
       </c>
       <c r="B22" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>64</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>65</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
@@ -2557,10 +2461,10 @@
         <v>29</v>
       </c>
       <c r="B23" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>67</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
@@ -2603,10 +2507,10 @@
         <v>29</v>
       </c>
       <c r="B24" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>68</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>69</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
@@ -2649,10 +2553,10 @@
         <v>29</v>
       </c>
       <c r="B25" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>70</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>71</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
@@ -2695,10 +2599,10 @@
         <v>29</v>
       </c>
       <c r="B26" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="10" t="s">
         <v>72</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>73</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
@@ -2741,10 +2645,10 @@
         <v>29</v>
       </c>
       <c r="B27" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>75</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
@@ -2787,10 +2691,10 @@
         <v>29</v>
       </c>
       <c r="B28" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>76</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>77</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
@@ -2833,7 +2737,7 @@
         <v>29</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>1</v>
+        <v>77</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>78</v>
@@ -2881,7 +2785,7 @@
       <c r="B30" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="11" t="s">
         <v>80</v>
       </c>
       <c r="D30" s="7"/>
@@ -2927,7 +2831,7 @@
       <c r="B31" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="11" t="s">
         <v>82</v>
       </c>
       <c r="D31" s="7"/>
@@ -2973,7 +2877,7 @@
       <c r="B32" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="11" t="s">
         <v>84</v>
       </c>
       <c r="D32" s="7"/>
@@ -3019,7 +2923,7 @@
       <c r="B33" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="11" t="s">
         <v>86</v>
       </c>
       <c r="D33" s="7"/>
@@ -3065,7 +2969,7 @@
       <c r="B34" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="11" t="s">
         <v>88</v>
       </c>
       <c r="D34" s="7"/>
@@ -3111,7 +3015,7 @@
       <c r="B35" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="11" t="s">
         <v>90</v>
       </c>
       <c r="D35" s="7"/>
@@ -3157,7 +3061,7 @@
       <c r="B36" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="11" t="s">
         <v>92</v>
       </c>
       <c r="D36" s="7"/>
@@ -3203,7 +3107,7 @@
       <c r="B37" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="11" t="s">
         <v>94</v>
       </c>
       <c r="D37" s="7"/>
@@ -3334,14 +3238,14 @@
       <c r="AK39" s="8"/>
       <c r="AL39" s="8"/>
     </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B40" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C40" s="11" t="s">
         <v>100</v>
       </c>
       <c r="D40" s="7"/>
@@ -3380,14 +3284,14 @@
       <c r="AK40" s="8"/>
       <c r="AL40" s="8"/>
     </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B41" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C41" s="11" t="s">
         <v>102</v>
       </c>
       <c r="D41" s="7"/>
@@ -3426,14 +3330,14 @@
       <c r="AK41" s="8"/>
       <c r="AL41" s="8"/>
     </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B42" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C42" s="11" t="s">
         <v>104</v>
       </c>
       <c r="D42" s="7"/>
@@ -3472,14 +3376,14 @@
       <c r="AK42" s="8"/>
       <c r="AL42" s="8"/>
     </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B43" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="11" t="s">
         <v>106</v>
       </c>
       <c r="D43" s="7"/>
@@ -3518,15 +3422,15 @@
       <c r="AK43" s="8"/>
       <c r="AL43" s="8"/>
     </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="C44" s="10" t="s">
-        <v>108</v>
+      <c r="C44" s="11" t="s">
+        <v>80</v>
       </c>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
@@ -3564,15 +3468,15 @@
       <c r="AK44" s="8"/>
       <c r="AL44" s="8"/>
     </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B45" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C45" s="11" t="s">
         <v>109</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>110</v>
       </c>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
@@ -3610,16 +3514,14 @@
       <c r="AK45" s="8"/>
       <c r="AL45" s="8"/>
     </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="7" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>112</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="C46" s="11"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
@@ -3656,16 +3558,12 @@
       <c r="AK46" s="8"/>
       <c r="AL46" s="8"/>
     </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="C47" s="11" t="s">
-        <v>114</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
@@ -3702,1547 +3600,863 @@
       <c r="AK47" s="8"/>
       <c r="AL47" s="8"/>
     </row>
-    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="7" t="s">
+    <row r="48" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B48" s="12"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="5"/>
+      <c r="Q48" s="5"/>
+      <c r="R48" s="5"/>
+      <c r="S48" s="5"/>
+      <c r="T48" s="5"/>
+      <c r="U48" s="5"/>
+      <c r="V48" s="5"/>
+      <c r="W48" s="5"/>
+      <c r="X48" s="5"/>
+      <c r="Y48" s="5"/>
+    </row>
+    <row r="49" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B49" s="12"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="5"/>
+      <c r="Q49" s="5"/>
+      <c r="R49" s="5"/>
+      <c r="S49" s="5"/>
+      <c r="T49" s="5"/>
+      <c r="U49" s="5"/>
+      <c r="V49" s="5"/>
+      <c r="W49" s="5"/>
+      <c r="X49" s="5"/>
+      <c r="Y49" s="5"/>
+    </row>
+    <row r="50" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="J50" s="13"/>
+      <c r="K50" s="13"/>
+      <c r="L50" s="13"/>
+      <c r="M50" s="13"/>
+      <c r="N50" s="13"/>
+      <c r="O50" s="13"/>
+      <c r="P50" s="13"/>
+      <c r="Q50" s="13"/>
+      <c r="R50" s="13"/>
+      <c r="S50" s="13"/>
+      <c r="T50" s="13"/>
+      <c r="U50" s="13"/>
+      <c r="V50" s="13"/>
+      <c r="W50" s="13"/>
+      <c r="X50" s="13"/>
+      <c r="Y50" s="13"/>
+      <c r="Z50" s="13"/>
+      <c r="AA50" s="13"/>
+      <c r="AB50" s="13"/>
+      <c r="AC50" s="13"/>
+      <c r="AD50" s="13"/>
+      <c r="AE50" s="13"/>
+      <c r="AF50" s="13"/>
+      <c r="AG50" s="13"/>
+      <c r="AH50" s="13"/>
+      <c r="AI50" s="13"/>
+      <c r="AJ50" s="13"/>
+      <c r="AK50" s="13"/>
+      <c r="AL50" s="13"/>
+    </row>
+    <row r="51" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="J51" s="13"/>
+      <c r="K51" s="13"/>
+      <c r="L51" s="13"/>
+      <c r="M51" s="13"/>
+      <c r="N51" s="13"/>
+      <c r="O51" s="13"/>
+      <c r="P51" s="13"/>
+      <c r="Q51" s="13"/>
+      <c r="R51" s="13"/>
+      <c r="S51" s="13"/>
+      <c r="T51" s="13"/>
+      <c r="U51" s="13"/>
+      <c r="V51" s="13"/>
+      <c r="W51" s="13"/>
+      <c r="X51" s="13"/>
+      <c r="Y51" s="13"/>
+      <c r="Z51" s="13"/>
+      <c r="AA51" s="13"/>
+      <c r="AB51" s="13"/>
+      <c r="AC51" s="13"/>
+      <c r="AD51" s="13"/>
+      <c r="AE51" s="13"/>
+      <c r="AF51" s="13"/>
+      <c r="AG51" s="13"/>
+      <c r="AH51" s="13"/>
+      <c r="AI51" s="13"/>
+      <c r="AJ51" s="13"/>
+      <c r="AK51" s="13"/>
+      <c r="AL51" s="13"/>
+    </row>
+    <row r="52" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="J52" s="13"/>
+      <c r="K52" s="13"/>
+      <c r="L52" s="13"/>
+      <c r="M52" s="13"/>
+      <c r="N52" s="13"/>
+      <c r="O52" s="13"/>
+      <c r="P52" s="13"/>
+      <c r="Q52" s="13"/>
+      <c r="R52" s="13"/>
+      <c r="S52" s="13"/>
+      <c r="T52" s="13"/>
+      <c r="U52" s="13"/>
+      <c r="V52" s="13"/>
+      <c r="W52" s="13"/>
+      <c r="X52" s="13"/>
+      <c r="Y52" s="13"/>
+      <c r="Z52" s="13"/>
+      <c r="AA52" s="13"/>
+      <c r="AB52" s="13"/>
+      <c r="AC52" s="13"/>
+      <c r="AD52" s="13"/>
+      <c r="AE52" s="13"/>
+      <c r="AF52" s="13"/>
+      <c r="AG52" s="13"/>
+      <c r="AH52" s="13"/>
+      <c r="AI52" s="13"/>
+      <c r="AJ52" s="13"/>
+      <c r="AK52" s="13"/>
+      <c r="AL52" s="13"/>
+    </row>
+    <row r="53" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="J53" s="13"/>
+      <c r="K53" s="13"/>
+      <c r="L53" s="13"/>
+      <c r="M53" s="13"/>
+      <c r="N53" s="13"/>
+      <c r="O53" s="13"/>
+      <c r="P53" s="16"/>
+      <c r="Q53" s="16"/>
+      <c r="R53" s="16"/>
+      <c r="S53" s="16"/>
+      <c r="T53" s="16"/>
+      <c r="U53" s="16"/>
+      <c r="V53" s="16"/>
+      <c r="W53" s="16"/>
+      <c r="X53" s="16"/>
+      <c r="Y53" s="16"/>
+      <c r="Z53" s="13"/>
+      <c r="AA53" s="13"/>
+      <c r="AB53" s="13"/>
+      <c r="AC53" s="13"/>
+      <c r="AD53" s="13"/>
+      <c r="AE53" s="13"/>
+      <c r="AF53" s="13"/>
+      <c r="AG53" s="13"/>
+      <c r="AH53" s="13"/>
+      <c r="AI53" s="13"/>
+      <c r="AJ53" s="13"/>
+      <c r="AK53" s="13"/>
+      <c r="AL53" s="13"/>
+    </row>
+    <row r="54" s="13" customFormat="true" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I54" s="13" t="str">
+        <f aca="true">TEXT(NOW(), "yyyy-mm-dd")</f>
+        <v>2020-08-26</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B48" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="7"/>
-      <c r="I48" s="7"/>
-      <c r="J48" s="7"/>
-      <c r="K48" s="7"/>
-      <c r="L48" s="7"/>
-      <c r="M48" s="7"/>
-      <c r="N48" s="7"/>
-      <c r="O48" s="8"/>
-      <c r="P48" s="8"/>
-      <c r="Q48" s="8"/>
-      <c r="R48" s="8"/>
-      <c r="S48" s="8"/>
-      <c r="T48" s="8"/>
-      <c r="U48" s="8"/>
-      <c r="V48" s="8"/>
-      <c r="W48" s="8"/>
-      <c r="X48" s="8"/>
-      <c r="Y48" s="8"/>
-      <c r="Z48" s="8"/>
-      <c r="AA48" s="8"/>
-      <c r="AB48" s="8"/>
-      <c r="AC48" s="8"/>
-      <c r="AD48" s="8"/>
-      <c r="AE48" s="8"/>
-      <c r="AF48" s="8"/>
-      <c r="AG48" s="8"/>
-      <c r="AH48" s="8"/>
-      <c r="AI48" s="8"/>
-      <c r="AJ48" s="8"/>
-      <c r="AK48" s="8"/>
-      <c r="AL48" s="8"/>
-    </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="7" t="s">
+      <c r="B55" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="17"/>
+      <c r="L55" s="13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="56" s="18" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B56" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="F56" s="18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="B57" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="C57" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="D57" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E57" s="21"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="H57" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="I57" s="22"/>
+      <c r="J57" s="22"/>
+      <c r="K57" s="19"/>
+      <c r="L57" s="19"/>
+      <c r="M57" s="22"/>
+      <c r="N57" s="19"/>
+      <c r="P57" s="23"/>
+      <c r="Q57" s="23"/>
+      <c r="U57" s="23"/>
+    </row>
+    <row r="58" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="B58" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="C58" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="D58" s="20"/>
+      <c r="E58" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F58" s="19"/>
+      <c r="G58" s="19"/>
+      <c r="H58" s="19"/>
+      <c r="I58" s="22"/>
+      <c r="J58" s="22"/>
+      <c r="K58" s="19"/>
+      <c r="L58" s="19"/>
+      <c r="M58" s="22"/>
+      <c r="N58" s="19"/>
+      <c r="P58" s="23"/>
+      <c r="Q58" s="23"/>
+      <c r="U58" s="23"/>
+    </row>
+    <row r="59" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="B59" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="D59" s="20"/>
+      <c r="E59" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="F59" s="19"/>
+      <c r="G59" s="19"/>
+      <c r="H59" s="19"/>
+      <c r="I59" s="22"/>
+      <c r="J59" s="22"/>
+      <c r="K59" s="19"/>
+      <c r="L59" s="19"/>
+      <c r="M59" s="22"/>
+      <c r="N59" s="19"/>
+      <c r="P59" s="23"/>
+      <c r="Q59" s="23"/>
+      <c r="U59" s="23"/>
+    </row>
+    <row r="60" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="B60" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="C60" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="D60" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E60" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F60" s="19"/>
+      <c r="G60" s="19"/>
+      <c r="H60" s="19"/>
+      <c r="I60" s="19"/>
+      <c r="J60" s="19"/>
+      <c r="K60" s="19"/>
+      <c r="L60" s="22"/>
+      <c r="M60" s="22"/>
+      <c r="N60" s="19"/>
+      <c r="P60" s="23"/>
+      <c r="Q60" s="23"/>
+      <c r="U60" s="23"/>
+    </row>
+    <row r="61" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B61" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="C61" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="D61" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E61" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="F61" s="19"/>
+      <c r="G61" s="19"/>
+      <c r="H61" s="19"/>
+      <c r="I61" s="19"/>
+      <c r="J61" s="19"/>
+      <c r="K61" s="19"/>
+      <c r="L61" s="22"/>
+      <c r="M61" s="22"/>
+      <c r="N61" s="19"/>
+      <c r="P61" s="23"/>
+      <c r="Q61" s="23"/>
+      <c r="U61" s="23"/>
+    </row>
+    <row r="62" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B62" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="C62" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="D62" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E62" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="F62" s="19"/>
+      <c r="G62" s="19"/>
+      <c r="H62" s="19"/>
+      <c r="I62" s="19"/>
+      <c r="J62" s="19"/>
+      <c r="K62" s="19"/>
+      <c r="L62" s="22"/>
+      <c r="M62" s="22"/>
+      <c r="N62" s="19"/>
+      <c r="P62" s="23"/>
+      <c r="Q62" s="23"/>
+      <c r="U62" s="23"/>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B63" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="C63" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="D63" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E63" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="F63" s="19"/>
+      <c r="G63" s="19"/>
+      <c r="H63" s="19"/>
+      <c r="I63" s="19"/>
+      <c r="J63" s="19"/>
+      <c r="K63" s="19"/>
+      <c r="L63" s="22"/>
+      <c r="M63" s="22"/>
+      <c r="N63" s="19"/>
+      <c r="P63" s="23"/>
+      <c r="Q63" s="23"/>
+      <c r="U63" s="23"/>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B64" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="C64" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="D64" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E64" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="F64" s="19"/>
+      <c r="G64" s="19"/>
+      <c r="H64" s="19"/>
+      <c r="I64" s="19"/>
+      <c r="J64" s="19"/>
+      <c r="K64" s="22"/>
+      <c r="L64" s="22"/>
+      <c r="M64" s="22"/>
+      <c r="N64" s="19"/>
+      <c r="P64" s="23"/>
+      <c r="Q64" s="23"/>
+      <c r="U64" s="23"/>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B65" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="C65" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="D65" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E65" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="F65" s="19"/>
+      <c r="G65" s="19"/>
+      <c r="H65" s="19"/>
+      <c r="I65" s="19"/>
+      <c r="J65" s="19"/>
+      <c r="K65" s="22"/>
+      <c r="L65" s="22"/>
+      <c r="M65" s="22"/>
+      <c r="N65" s="19"/>
+      <c r="P65" s="23"/>
+      <c r="Q65" s="23"/>
+      <c r="U65" s="23"/>
+    </row>
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="27"/>
+      <c r="G66" s="28"/>
+      <c r="H66" s="28"/>
+      <c r="I66" s="28"/>
+      <c r="J66" s="28"/>
+      <c r="K66" s="28"/>
+      <c r="L66" s="28"/>
+      <c r="M66" s="28"/>
+      <c r="N66" s="28"/>
+    </row>
+    <row r="67" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B67" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="C67" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="D67" s="20"/>
+      <c r="E67" s="24"/>
+      <c r="F67" s="19"/>
+      <c r="G67" s="19"/>
+      <c r="H67" s="19"/>
+      <c r="I67" s="19"/>
+      <c r="J67" s="19"/>
+      <c r="K67" s="22"/>
+      <c r="L67" s="22"/>
+      <c r="M67" s="22"/>
+      <c r="N67" s="19"/>
+      <c r="P67" s="23"/>
+      <c r="Q67" s="23"/>
+      <c r="U67" s="23"/>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
+      <c r="H68" s="6"/>
+      <c r="I68" s="6"/>
+      <c r="J68" s="6"/>
+      <c r="K68" s="6"/>
+      <c r="L68" s="6"/>
+      <c r="M68" s="6"/>
+      <c r="N68" s="6"/>
+    </row>
+    <row r="69" s="25" customFormat="true" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B49" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="7"/>
-      <c r="H49" s="7"/>
-      <c r="I49" s="7"/>
-      <c r="J49" s="7"/>
-      <c r="K49" s="7"/>
-      <c r="L49" s="7"/>
-      <c r="M49" s="7"/>
-      <c r="N49" s="7"/>
-      <c r="O49" s="8"/>
-      <c r="P49" s="8"/>
-      <c r="Q49" s="8"/>
-      <c r="R49" s="8"/>
-      <c r="S49" s="8"/>
-      <c r="T49" s="8"/>
-      <c r="U49" s="8"/>
-      <c r="V49" s="8"/>
-      <c r="W49" s="8"/>
-      <c r="X49" s="8"/>
-      <c r="Y49" s="8"/>
-      <c r="Z49" s="8"/>
-      <c r="AA49" s="8"/>
-      <c r="AB49" s="8"/>
-      <c r="AC49" s="8"/>
-      <c r="AD49" s="8"/>
-      <c r="AE49" s="8"/>
-      <c r="AF49" s="8"/>
-      <c r="AG49" s="8"/>
-      <c r="AH49" s="8"/>
-      <c r="AI49" s="8"/>
-      <c r="AJ49" s="8"/>
-      <c r="AK49" s="8"/>
-      <c r="AL49" s="8"/>
-    </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="7" t="s">
+      <c r="B69" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="C69" s="20"/>
+      <c r="D69" s="19"/>
+      <c r="E69" s="21"/>
+      <c r="F69" s="19"/>
+      <c r="G69" s="19"/>
+      <c r="H69" s="19"/>
+      <c r="I69" s="22"/>
+      <c r="J69" s="19"/>
+      <c r="K69" s="19"/>
+      <c r="L69" s="22"/>
+      <c r="M69" s="22"/>
+      <c r="N69" s="19"/>
+      <c r="P69" s="23"/>
+      <c r="Q69" s="23"/>
+      <c r="U69" s="23"/>
+    </row>
+    <row r="70" s="18" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B71" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="C71" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D71" s="27"/>
+      <c r="E71" s="27"/>
+      <c r="F71" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B50" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="7"/>
-      <c r="H50" s="7"/>
-      <c r="I50" s="7"/>
-      <c r="J50" s="7"/>
-      <c r="K50" s="7"/>
-      <c r="L50" s="7"/>
-      <c r="M50" s="7"/>
-      <c r="N50" s="7"/>
-      <c r="O50" s="8"/>
-      <c r="P50" s="8"/>
-      <c r="Q50" s="8"/>
-      <c r="R50" s="8"/>
-      <c r="S50" s="8"/>
-      <c r="T50" s="8"/>
-      <c r="U50" s="8"/>
-      <c r="V50" s="8"/>
-      <c r="W50" s="8"/>
-      <c r="X50" s="8"/>
-      <c r="Y50" s="8"/>
-      <c r="Z50" s="8"/>
-      <c r="AA50" s="8"/>
-      <c r="AB50" s="8"/>
-      <c r="AC50" s="8"/>
-      <c r="AD50" s="8"/>
-      <c r="AE50" s="8"/>
-      <c r="AF50" s="8"/>
-      <c r="AG50" s="8"/>
-      <c r="AH50" s="8"/>
-      <c r="AI50" s="8"/>
-      <c r="AJ50" s="8"/>
-      <c r="AK50" s="8"/>
-      <c r="AL50" s="8"/>
-    </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B51" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="7"/>
-      <c r="H51" s="7"/>
-      <c r="I51" s="7"/>
-      <c r="J51" s="7"/>
-      <c r="K51" s="7"/>
-      <c r="L51" s="7"/>
-      <c r="M51" s="7"/>
-      <c r="N51" s="7"/>
-      <c r="O51" s="8"/>
-      <c r="P51" s="8"/>
-      <c r="Q51" s="8"/>
-      <c r="R51" s="8"/>
-      <c r="S51" s="8"/>
-      <c r="T51" s="8"/>
-      <c r="U51" s="8"/>
-      <c r="V51" s="8"/>
-      <c r="W51" s="8"/>
-      <c r="X51" s="8"/>
-      <c r="Y51" s="8"/>
-      <c r="Z51" s="8"/>
-      <c r="AA51" s="8"/>
-      <c r="AB51" s="8"/>
-      <c r="AC51" s="8"/>
-      <c r="AD51" s="8"/>
-      <c r="AE51" s="8"/>
-      <c r="AF51" s="8"/>
-      <c r="AG51" s="8"/>
-      <c r="AH51" s="8"/>
-      <c r="AI51" s="8"/>
-      <c r="AJ51" s="8"/>
-      <c r="AK51" s="8"/>
-      <c r="AL51" s="8"/>
-    </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B52" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="D52" s="7"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="7"/>
-      <c r="G52" s="7"/>
-      <c r="H52" s="7"/>
-      <c r="I52" s="7"/>
-      <c r="J52" s="7"/>
-      <c r="K52" s="7"/>
-      <c r="L52" s="7"/>
-      <c r="M52" s="7"/>
-      <c r="N52" s="7"/>
-      <c r="O52" s="8"/>
-      <c r="P52" s="8"/>
-      <c r="Q52" s="8"/>
-      <c r="R52" s="8"/>
-      <c r="S52" s="8"/>
-      <c r="T52" s="8"/>
-      <c r="U52" s="8"/>
-      <c r="V52" s="8"/>
-      <c r="W52" s="8"/>
-      <c r="X52" s="8"/>
-      <c r="Y52" s="8"/>
-      <c r="Z52" s="8"/>
-      <c r="AA52" s="8"/>
-      <c r="AB52" s="8"/>
-      <c r="AC52" s="8"/>
-      <c r="AD52" s="8"/>
-      <c r="AE52" s="8"/>
-      <c r="AF52" s="8"/>
-      <c r="AG52" s="8"/>
-      <c r="AH52" s="8"/>
-      <c r="AI52" s="8"/>
-      <c r="AJ52" s="8"/>
-      <c r="AK52" s="8"/>
-      <c r="AL52" s="8"/>
-    </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B53" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="C53" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
-      <c r="G53" s="7"/>
-      <c r="H53" s="7"/>
-      <c r="I53" s="7"/>
-      <c r="J53" s="7"/>
-      <c r="K53" s="7"/>
-      <c r="L53" s="7"/>
-      <c r="M53" s="7"/>
-      <c r="N53" s="7"/>
-      <c r="O53" s="8"/>
-      <c r="P53" s="8"/>
-      <c r="Q53" s="8"/>
-      <c r="R53" s="8"/>
-      <c r="S53" s="8"/>
-      <c r="T53" s="8"/>
-      <c r="U53" s="8"/>
-      <c r="V53" s="8"/>
-      <c r="W53" s="8"/>
-      <c r="X53" s="8"/>
-      <c r="Y53" s="8"/>
-      <c r="Z53" s="8"/>
-      <c r="AA53" s="8"/>
-      <c r="AB53" s="8"/>
-      <c r="AC53" s="8"/>
-      <c r="AD53" s="8"/>
-      <c r="AE53" s="8"/>
-      <c r="AF53" s="8"/>
-      <c r="AG53" s="8"/>
-      <c r="AH53" s="8"/>
-      <c r="AI53" s="8"/>
-      <c r="AJ53" s="8"/>
-      <c r="AK53" s="8"/>
-      <c r="AL53" s="8"/>
-    </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B54" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C54" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="7"/>
-      <c r="G54" s="7"/>
-      <c r="H54" s="7"/>
-      <c r="I54" s="7"/>
-      <c r="J54" s="7"/>
-      <c r="K54" s="7"/>
-      <c r="L54" s="7"/>
-      <c r="M54" s="7"/>
-      <c r="N54" s="7"/>
-      <c r="O54" s="8"/>
-      <c r="P54" s="8"/>
-      <c r="Q54" s="8"/>
-      <c r="R54" s="8"/>
-      <c r="S54" s="8"/>
-      <c r="T54" s="8"/>
-      <c r="U54" s="8"/>
-      <c r="V54" s="8"/>
-      <c r="W54" s="8"/>
-      <c r="X54" s="8"/>
-      <c r="Y54" s="8"/>
-      <c r="Z54" s="8"/>
-      <c r="AA54" s="8"/>
-      <c r="AB54" s="8"/>
-      <c r="AC54" s="8"/>
-      <c r="AD54" s="8"/>
-      <c r="AE54" s="8"/>
-      <c r="AF54" s="8"/>
-      <c r="AG54" s="8"/>
-      <c r="AH54" s="8"/>
-      <c r="AI54" s="8"/>
-      <c r="AJ54" s="8"/>
-      <c r="AK54" s="8"/>
-      <c r="AL54" s="8"/>
-    </row>
-    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B55" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="C55" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="7"/>
-      <c r="H55" s="7"/>
-      <c r="I55" s="7"/>
-      <c r="J55" s="7"/>
-      <c r="K55" s="7"/>
-      <c r="L55" s="7"/>
-      <c r="M55" s="7"/>
-      <c r="N55" s="7"/>
-      <c r="O55" s="8"/>
-      <c r="P55" s="8"/>
-      <c r="Q55" s="8"/>
-      <c r="R55" s="8"/>
-      <c r="S55" s="8"/>
-      <c r="T55" s="8"/>
-      <c r="U55" s="8"/>
-      <c r="V55" s="8"/>
-      <c r="W55" s="8"/>
-      <c r="X55" s="8"/>
-      <c r="Y55" s="8"/>
-      <c r="Z55" s="8"/>
-      <c r="AA55" s="8"/>
-      <c r="AB55" s="8"/>
-      <c r="AC55" s="8"/>
-      <c r="AD55" s="8"/>
-      <c r="AE55" s="8"/>
-      <c r="AF55" s="8"/>
-      <c r="AG55" s="8"/>
-      <c r="AH55" s="8"/>
-      <c r="AI55" s="8"/>
-      <c r="AJ55" s="8"/>
-      <c r="AK55" s="8"/>
-      <c r="AL55" s="8"/>
-    </row>
-    <row r="56" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B56" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="D56" s="7"/>
-      <c r="E56" s="7"/>
-      <c r="F56" s="7"/>
-      <c r="G56" s="7"/>
-      <c r="H56" s="7"/>
-      <c r="I56" s="7"/>
-      <c r="J56" s="7"/>
-      <c r="K56" s="7"/>
-      <c r="L56" s="7"/>
-      <c r="M56" s="7"/>
-      <c r="N56" s="7"/>
-      <c r="O56" s="8"/>
-      <c r="P56" s="8"/>
-      <c r="Q56" s="8"/>
-      <c r="R56" s="8"/>
-      <c r="S56" s="8"/>
-      <c r="T56" s="8"/>
-      <c r="U56" s="8"/>
-      <c r="V56" s="8"/>
-      <c r="W56" s="8"/>
-      <c r="X56" s="8"/>
-      <c r="Y56" s="8"/>
-      <c r="Z56" s="8"/>
-      <c r="AA56" s="8"/>
-      <c r="AB56" s="8"/>
-      <c r="AC56" s="8"/>
-      <c r="AD56" s="8"/>
-      <c r="AE56" s="8"/>
-      <c r="AF56" s="8"/>
-      <c r="AG56" s="8"/>
-      <c r="AH56" s="8"/>
-      <c r="AI56" s="8"/>
-      <c r="AJ56" s="8"/>
-      <c r="AK56" s="8"/>
-      <c r="AL56" s="8"/>
-    </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B57" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="C57" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="D57" s="7"/>
-      <c r="E57" s="7"/>
-      <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
-      <c r="H57" s="7"/>
-      <c r="I57" s="7"/>
-      <c r="J57" s="7"/>
-      <c r="K57" s="7"/>
-      <c r="L57" s="7"/>
-      <c r="M57" s="7"/>
-      <c r="N57" s="7"/>
-      <c r="O57" s="8"/>
-      <c r="P57" s="8"/>
-      <c r="Q57" s="8"/>
-      <c r="R57" s="8"/>
-      <c r="S57" s="8"/>
-      <c r="T57" s="8"/>
-      <c r="U57" s="8"/>
-      <c r="V57" s="8"/>
-      <c r="W57" s="8"/>
-      <c r="X57" s="8"/>
-      <c r="Y57" s="8"/>
-      <c r="Z57" s="8"/>
-      <c r="AA57" s="8"/>
-      <c r="AB57" s="8"/>
-      <c r="AC57" s="8"/>
-      <c r="AD57" s="8"/>
-      <c r="AE57" s="8"/>
-      <c r="AF57" s="8"/>
-      <c r="AG57" s="8"/>
-      <c r="AH57" s="8"/>
-      <c r="AI57" s="8"/>
-      <c r="AJ57" s="8"/>
-      <c r="AK57" s="8"/>
-      <c r="AL57" s="8"/>
-    </row>
-    <row r="58" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B58" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="C58" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D58" s="7"/>
-      <c r="E58" s="7"/>
-      <c r="F58" s="7"/>
-      <c r="G58" s="7"/>
-      <c r="H58" s="7"/>
-      <c r="I58" s="7"/>
-      <c r="J58" s="7"/>
-      <c r="K58" s="7"/>
-      <c r="L58" s="7"/>
-      <c r="M58" s="7"/>
-      <c r="N58" s="7"/>
-      <c r="O58" s="8"/>
-      <c r="P58" s="8"/>
-      <c r="Q58" s="8"/>
-      <c r="R58" s="8"/>
-      <c r="S58" s="8"/>
-      <c r="T58" s="8"/>
-      <c r="U58" s="8"/>
-      <c r="V58" s="8"/>
-      <c r="W58" s="8"/>
-      <c r="X58" s="8"/>
-      <c r="Y58" s="8"/>
-      <c r="Z58" s="8"/>
-      <c r="AA58" s="8"/>
-      <c r="AB58" s="8"/>
-      <c r="AC58" s="8"/>
-      <c r="AD58" s="8"/>
-      <c r="AE58" s="8"/>
-      <c r="AF58" s="8"/>
-      <c r="AG58" s="8"/>
-      <c r="AH58" s="8"/>
-      <c r="AI58" s="8"/>
-      <c r="AJ58" s="8"/>
-      <c r="AK58" s="8"/>
-      <c r="AL58" s="8"/>
-    </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B59" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="C59" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="D59" s="7"/>
-      <c r="E59" s="7"/>
-      <c r="F59" s="7"/>
-      <c r="G59" s="7"/>
-      <c r="H59" s="7"/>
-      <c r="I59" s="7"/>
-      <c r="J59" s="7"/>
-      <c r="K59" s="7"/>
-      <c r="L59" s="7"/>
-      <c r="M59" s="7"/>
-      <c r="N59" s="7"/>
-      <c r="O59" s="8"/>
-      <c r="P59" s="8"/>
-      <c r="Q59" s="8"/>
-      <c r="R59" s="8"/>
-      <c r="S59" s="8"/>
-      <c r="T59" s="8"/>
-      <c r="U59" s="8"/>
-      <c r="V59" s="8"/>
-      <c r="W59" s="8"/>
-      <c r="X59" s="8"/>
-      <c r="Y59" s="8"/>
-      <c r="Z59" s="8"/>
-      <c r="AA59" s="8"/>
-      <c r="AB59" s="8"/>
-      <c r="AC59" s="8"/>
-      <c r="AD59" s="8"/>
-      <c r="AE59" s="8"/>
-      <c r="AF59" s="8"/>
-      <c r="AG59" s="8"/>
-      <c r="AH59" s="8"/>
-      <c r="AI59" s="8"/>
-      <c r="AJ59" s="8"/>
-      <c r="AK59" s="8"/>
-      <c r="AL59" s="8"/>
-    </row>
-    <row r="60" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B60" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="C60" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="7"/>
-      <c r="G60" s="7"/>
-      <c r="H60" s="7"/>
-      <c r="I60" s="7"/>
-      <c r="J60" s="7"/>
-      <c r="K60" s="7"/>
-      <c r="L60" s="7"/>
-      <c r="M60" s="7"/>
-      <c r="N60" s="7"/>
-      <c r="O60" s="8"/>
-      <c r="P60" s="8"/>
-      <c r="Q60" s="8"/>
-      <c r="R60" s="8"/>
-      <c r="S60" s="8"/>
-      <c r="T60" s="8"/>
-      <c r="U60" s="8"/>
-      <c r="V60" s="8"/>
-      <c r="W60" s="8"/>
-      <c r="X60" s="8"/>
-      <c r="Y60" s="8"/>
-      <c r="Z60" s="8"/>
-      <c r="AA60" s="8"/>
-      <c r="AB60" s="8"/>
-      <c r="AC60" s="8"/>
-      <c r="AD60" s="8"/>
-      <c r="AE60" s="8"/>
-      <c r="AF60" s="8"/>
-      <c r="AG60" s="8"/>
-      <c r="AH60" s="8"/>
-      <c r="AI60" s="8"/>
-      <c r="AJ60" s="8"/>
-      <c r="AK60" s="8"/>
-      <c r="AL60" s="8"/>
-    </row>
-    <row r="61" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B61" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="C61" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="D61" s="7"/>
-      <c r="E61" s="7"/>
-      <c r="F61" s="7"/>
-      <c r="G61" s="7"/>
-      <c r="H61" s="7"/>
-      <c r="I61" s="7"/>
-      <c r="J61" s="7"/>
-      <c r="K61" s="7"/>
-      <c r="L61" s="7"/>
-      <c r="M61" s="7"/>
-      <c r="N61" s="7"/>
-      <c r="O61" s="8"/>
-      <c r="P61" s="8"/>
-      <c r="Q61" s="8"/>
-      <c r="R61" s="8"/>
-      <c r="S61" s="8"/>
-      <c r="T61" s="8"/>
-      <c r="U61" s="8"/>
-      <c r="V61" s="8"/>
-      <c r="W61" s="8"/>
-      <c r="X61" s="8"/>
-      <c r="Y61" s="8"/>
-      <c r="Z61" s="8"/>
-      <c r="AA61" s="8"/>
-      <c r="AB61" s="8"/>
-      <c r="AC61" s="8"/>
-      <c r="AD61" s="8"/>
-      <c r="AE61" s="8"/>
-      <c r="AF61" s="8"/>
-      <c r="AG61" s="8"/>
-      <c r="AH61" s="8"/>
-      <c r="AI61" s="8"/>
-      <c r="AJ61" s="8"/>
-      <c r="AK61" s="8"/>
-      <c r="AL61" s="8"/>
-    </row>
-    <row r="62" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B62" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="C62" s="11"/>
-      <c r="D62" s="7"/>
-      <c r="E62" s="7"/>
-      <c r="F62" s="7"/>
-      <c r="G62" s="7"/>
-      <c r="H62" s="7"/>
-      <c r="I62" s="7"/>
-      <c r="J62" s="7"/>
-      <c r="K62" s="7"/>
-      <c r="L62" s="7"/>
-      <c r="M62" s="7"/>
-      <c r="N62" s="7"/>
-      <c r="O62" s="8"/>
-      <c r="P62" s="8"/>
-      <c r="Q62" s="8"/>
-      <c r="R62" s="8"/>
-      <c r="S62" s="8"/>
-      <c r="T62" s="8"/>
-      <c r="U62" s="8"/>
-      <c r="V62" s="8"/>
-      <c r="W62" s="8"/>
-      <c r="X62" s="8"/>
-      <c r="Y62" s="8"/>
-      <c r="Z62" s="8"/>
-      <c r="AA62" s="8"/>
-      <c r="AB62" s="8"/>
-      <c r="AC62" s="8"/>
-      <c r="AD62" s="8"/>
-      <c r="AE62" s="8"/>
-      <c r="AF62" s="8"/>
-      <c r="AG62" s="8"/>
-      <c r="AH62" s="8"/>
-      <c r="AI62" s="8"/>
-      <c r="AJ62" s="8"/>
-      <c r="AK62" s="8"/>
-      <c r="AL62" s="8"/>
-    </row>
-    <row r="63" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="7" t="s">
+      <c r="G71" s="27"/>
+      <c r="H71" s="27"/>
+      <c r="I71" s="27"/>
+      <c r="J71" s="27"/>
+      <c r="K71" s="27"/>
+      <c r="L71" s="27"/>
+      <c r="M71" s="27"/>
+      <c r="N71" s="27"/>
+    </row>
+    <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D72" s="28"/>
+      <c r="E72" s="31"/>
+      <c r="F72" s="31"/>
+      <c r="G72" s="31"/>
+      <c r="H72" s="31"/>
+      <c r="I72" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="J72" s="31"/>
+      <c r="K72" s="31"/>
+      <c r="L72" s="31"/>
+      <c r="M72" s="31"/>
+      <c r="N72" s="31"/>
+    </row>
+    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="B63" s="11"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="7"/>
-      <c r="E63" s="7"/>
-      <c r="F63" s="7"/>
-      <c r="G63" s="7"/>
-      <c r="H63" s="7"/>
-      <c r="I63" s="7"/>
-      <c r="J63" s="7"/>
-      <c r="K63" s="7"/>
-      <c r="L63" s="7"/>
-      <c r="M63" s="7"/>
-      <c r="N63" s="7"/>
-      <c r="O63" s="8"/>
-      <c r="P63" s="8"/>
-      <c r="Q63" s="8"/>
-      <c r="R63" s="8"/>
-      <c r="S63" s="8"/>
-      <c r="T63" s="8"/>
-      <c r="U63" s="8"/>
-      <c r="V63" s="8"/>
-      <c r="W63" s="8"/>
-      <c r="X63" s="8"/>
-      <c r="Y63" s="8"/>
-      <c r="Z63" s="8"/>
-      <c r="AA63" s="8"/>
-      <c r="AB63" s="8"/>
-      <c r="AC63" s="8"/>
-      <c r="AD63" s="8"/>
-      <c r="AE63" s="8"/>
-      <c r="AF63" s="8"/>
-      <c r="AG63" s="8"/>
-      <c r="AH63" s="8"/>
-      <c r="AI63" s="8"/>
-      <c r="AJ63" s="8"/>
-      <c r="AK63" s="8"/>
-      <c r="AL63" s="8"/>
-    </row>
-    <row r="64" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B64" s="12"/>
-      <c r="C64" s="12"/>
-      <c r="D64" s="4"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="4"/>
-      <c r="G64" s="4"/>
-      <c r="H64" s="4"/>
-      <c r="I64" s="4"/>
-      <c r="J64" s="4"/>
-      <c r="K64" s="4"/>
-      <c r="L64" s="4"/>
-      <c r="M64" s="4"/>
-      <c r="N64" s="4"/>
-      <c r="O64" s="4"/>
-      <c r="P64" s="5"/>
-      <c r="Q64" s="5"/>
-      <c r="R64" s="5"/>
-      <c r="S64" s="5"/>
-      <c r="T64" s="5"/>
-      <c r="U64" s="5"/>
-      <c r="V64" s="5"/>
-      <c r="W64" s="5"/>
-      <c r="X64" s="5"/>
-      <c r="Y64" s="5"/>
-    </row>
-    <row r="65" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B65" s="12"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="4"/>
-      <c r="G65" s="4"/>
-      <c r="H65" s="4"/>
-      <c r="I65" s="4"/>
-      <c r="J65" s="4"/>
-      <c r="K65" s="4"/>
-      <c r="L65" s="4"/>
-      <c r="M65" s="4"/>
-      <c r="N65" s="4"/>
-      <c r="O65" s="4"/>
-      <c r="P65" s="5"/>
-      <c r="Q65" s="5"/>
-      <c r="R65" s="5"/>
-      <c r="S65" s="5"/>
-      <c r="T65" s="5"/>
-      <c r="U65" s="5"/>
-      <c r="V65" s="5"/>
-      <c r="W65" s="5"/>
-      <c r="X65" s="5"/>
-      <c r="Y65" s="5"/>
-    </row>
-    <row r="66" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="13" t="s">
+      <c r="B73" s="27"/>
+      <c r="C73" s="27"/>
+      <c r="D73" s="27"/>
+      <c r="E73" s="27"/>
+      <c r="F73" s="27"/>
+      <c r="G73" s="27"/>
+      <c r="H73" s="27"/>
+      <c r="I73" s="27"/>
+      <c r="J73" s="27"/>
+      <c r="K73" s="27"/>
+      <c r="L73" s="27"/>
+      <c r="M73" s="27"/>
+      <c r="N73" s="27"/>
+    </row>
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B66" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="C66" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D66" s="13"/>
-      <c r="E66" s="13"/>
-      <c r="F66" s="13"/>
-      <c r="G66" s="13"/>
-      <c r="H66" s="13"/>
-      <c r="I66" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="J66" s="13"/>
-      <c r="K66" s="13"/>
-      <c r="L66" s="13"/>
-      <c r="M66" s="13"/>
-      <c r="N66" s="13"/>
-      <c r="O66" s="13"/>
-      <c r="P66" s="13"/>
-      <c r="Q66" s="13"/>
-      <c r="R66" s="13"/>
-      <c r="S66" s="13"/>
-      <c r="T66" s="13"/>
-      <c r="U66" s="13"/>
-      <c r="V66" s="13"/>
-      <c r="W66" s="13"/>
-      <c r="X66" s="13"/>
-      <c r="Y66" s="13"/>
-      <c r="Z66" s="13"/>
-      <c r="AA66" s="13"/>
-      <c r="AB66" s="13"/>
-      <c r="AC66" s="13"/>
-      <c r="AD66" s="13"/>
-      <c r="AE66" s="13"/>
-      <c r="AF66" s="13"/>
-      <c r="AG66" s="13"/>
-      <c r="AH66" s="13"/>
-      <c r="AI66" s="13"/>
-      <c r="AJ66" s="13"/>
-      <c r="AK66" s="13"/>
-      <c r="AL66" s="13"/>
-    </row>
-    <row r="67" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B67" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="C67" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D67" s="13"/>
-      <c r="E67" s="13"/>
-      <c r="F67" s="13"/>
-      <c r="G67" s="13"/>
-      <c r="H67" s="13"/>
-      <c r="I67" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="J67" s="13"/>
-      <c r="K67" s="13"/>
-      <c r="L67" s="13"/>
-      <c r="M67" s="13"/>
-      <c r="N67" s="13"/>
-      <c r="O67" s="13"/>
-      <c r="P67" s="13"/>
-      <c r="Q67" s="13"/>
-      <c r="R67" s="13"/>
-      <c r="S67" s="13"/>
-      <c r="T67" s="13"/>
-      <c r="U67" s="13"/>
-      <c r="V67" s="13"/>
-      <c r="W67" s="13"/>
-      <c r="X67" s="13"/>
-      <c r="Y67" s="13"/>
-      <c r="Z67" s="13"/>
-      <c r="AA67" s="13"/>
-      <c r="AB67" s="13"/>
-      <c r="AC67" s="13"/>
-      <c r="AD67" s="13"/>
-      <c r="AE67" s="13"/>
-      <c r="AF67" s="13"/>
-      <c r="AG67" s="13"/>
-      <c r="AH67" s="13"/>
-      <c r="AI67" s="13"/>
-      <c r="AJ67" s="13"/>
-      <c r="AK67" s="13"/>
-      <c r="AL67" s="13"/>
-    </row>
-    <row r="68" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B68" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="C68" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D68" s="13"/>
-      <c r="E68" s="13"/>
-      <c r="F68" s="13"/>
-      <c r="G68" s="13"/>
-      <c r="H68" s="13"/>
-      <c r="I68" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="J68" s="13"/>
-      <c r="K68" s="13"/>
-      <c r="L68" s="13"/>
-      <c r="M68" s="13"/>
-      <c r="N68" s="13"/>
-      <c r="O68" s="13"/>
-      <c r="P68" s="13"/>
-      <c r="Q68" s="13"/>
-      <c r="R68" s="13"/>
-      <c r="S68" s="13"/>
-      <c r="T68" s="13"/>
-      <c r="U68" s="13"/>
-      <c r="V68" s="13"/>
-      <c r="W68" s="13"/>
-      <c r="X68" s="13"/>
-      <c r="Y68" s="13"/>
-      <c r="Z68" s="13"/>
-      <c r="AA68" s="13"/>
-      <c r="AB68" s="13"/>
-      <c r="AC68" s="13"/>
-      <c r="AD68" s="13"/>
-      <c r="AE68" s="13"/>
-      <c r="AF68" s="13"/>
-      <c r="AG68" s="13"/>
-      <c r="AH68" s="13"/>
-      <c r="AI68" s="13"/>
-      <c r="AJ68" s="13"/>
-      <c r="AK68" s="13"/>
-      <c r="AL68" s="13"/>
-    </row>
-    <row r="69" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B69" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="C69" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D69" s="13"/>
-      <c r="E69" s="13"/>
-      <c r="F69" s="13"/>
-      <c r="G69" s="13"/>
-      <c r="H69" s="13"/>
-      <c r="I69" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="J69" s="13"/>
-      <c r="K69" s="13"/>
-      <c r="L69" s="13"/>
-      <c r="M69" s="13"/>
-      <c r="N69" s="13"/>
-      <c r="O69" s="13"/>
-      <c r="P69" s="16"/>
-      <c r="Q69" s="16"/>
-      <c r="R69" s="16"/>
-      <c r="S69" s="16"/>
-      <c r="T69" s="16"/>
-      <c r="U69" s="16"/>
-      <c r="V69" s="16"/>
-      <c r="W69" s="16"/>
-      <c r="X69" s="16"/>
-      <c r="Y69" s="16"/>
-      <c r="Z69" s="13"/>
-      <c r="AA69" s="13"/>
-      <c r="AB69" s="13"/>
-      <c r="AC69" s="13"/>
-      <c r="AD69" s="13"/>
-      <c r="AE69" s="13"/>
-      <c r="AF69" s="13"/>
-      <c r="AG69" s="13"/>
-      <c r="AH69" s="13"/>
-      <c r="AI69" s="13"/>
-      <c r="AJ69" s="13"/>
-      <c r="AK69" s="13"/>
-      <c r="AL69" s="13"/>
-    </row>
-    <row r="70" s="13" customFormat="true" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B70" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="C70" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="I70" s="13" t="str">
-        <f aca="true">TEXT(NOW(), "yyyy-mm-dd")</f>
-        <v>2020-08-25</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B71" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="C71" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D71" s="13"/>
-      <c r="E71" s="13"/>
-      <c r="F71" s="13"/>
-      <c r="G71" s="13"/>
-      <c r="H71" s="13"/>
-      <c r="I71" s="17"/>
-      <c r="L71" s="13" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="72" s="18" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B72" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="C72" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="F72" s="18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="B73" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="C73" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="D73" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="E73" s="21"/>
-      <c r="F73" s="19"/>
-      <c r="G73" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="H73" s="19" t="s">
-        <v>160</v>
-      </c>
-      <c r="I73" s="22"/>
-      <c r="J73" s="22"/>
-      <c r="K73" s="19"/>
-      <c r="L73" s="19"/>
-      <c r="M73" s="22"/>
-      <c r="N73" s="19"/>
-      <c r="P73" s="23"/>
-      <c r="Q73" s="23"/>
-      <c r="U73" s="23"/>
-    </row>
-    <row r="74" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="B74" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="C74" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="D74" s="20"/>
-      <c r="E74" s="24" t="s">
+      <c r="B74" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="F74" s="19"/>
-      <c r="G74" s="19"/>
-      <c r="H74" s="19"/>
-      <c r="I74" s="22"/>
-      <c r="J74" s="22"/>
-      <c r="K74" s="19"/>
-      <c r="L74" s="19"/>
-      <c r="M74" s="22"/>
-      <c r="N74" s="19"/>
-      <c r="P74" s="23"/>
-      <c r="Q74" s="23"/>
-      <c r="U74" s="23"/>
-    </row>
-    <row r="75" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="B75" s="20" t="s">
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="7"/>
+      <c r="F74" s="7"/>
+      <c r="G74" s="7"/>
+      <c r="H74" s="7"/>
+      <c r="I74" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="C75" s="20" t="s">
-        <v>166</v>
-      </c>
-      <c r="D75" s="20"/>
-      <c r="E75" s="24" t="s">
-        <v>167</v>
-      </c>
-      <c r="F75" s="19"/>
-      <c r="G75" s="19"/>
-      <c r="H75" s="19"/>
-      <c r="I75" s="22"/>
-      <c r="J75" s="22"/>
-      <c r="K75" s="19"/>
-      <c r="L75" s="19"/>
-      <c r="M75" s="22"/>
-      <c r="N75" s="19"/>
-      <c r="P75" s="23"/>
-      <c r="Q75" s="23"/>
-      <c r="U75" s="23"/>
-    </row>
-    <row r="76" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="B76" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="C76" s="20" t="s">
-        <v>170</v>
-      </c>
-      <c r="D76" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E76" s="24" t="s">
-        <v>164</v>
-      </c>
-      <c r="F76" s="19"/>
-      <c r="G76" s="19"/>
-      <c r="H76" s="19"/>
-      <c r="I76" s="19"/>
-      <c r="J76" s="19"/>
-      <c r="K76" s="19"/>
-      <c r="L76" s="22"/>
-      <c r="M76" s="22"/>
-      <c r="N76" s="19"/>
-      <c r="P76" s="23"/>
-      <c r="Q76" s="23"/>
-      <c r="U76" s="23"/>
-    </row>
-    <row r="77" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="B77" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="C77" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="D77" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E77" s="24" t="s">
-        <v>174</v>
-      </c>
-      <c r="F77" s="19"/>
-      <c r="G77" s="19"/>
-      <c r="H77" s="19"/>
-      <c r="I77" s="19"/>
-      <c r="J77" s="19"/>
-      <c r="K77" s="19"/>
-      <c r="L77" s="22"/>
-      <c r="M77" s="22"/>
-      <c r="N77" s="19"/>
-      <c r="P77" s="23"/>
-      <c r="Q77" s="23"/>
-      <c r="U77" s="23"/>
-    </row>
-    <row r="78" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="B78" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="C78" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="D78" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E78" s="24" t="s">
-        <v>178</v>
-      </c>
-      <c r="F78" s="19"/>
-      <c r="G78" s="19"/>
-      <c r="H78" s="19"/>
-      <c r="I78" s="19"/>
-      <c r="J78" s="19"/>
-      <c r="K78" s="19"/>
-      <c r="L78" s="22"/>
-      <c r="M78" s="22"/>
-      <c r="N78" s="19"/>
-      <c r="P78" s="23"/>
-      <c r="Q78" s="23"/>
-      <c r="U78" s="23"/>
-    </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="B79" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="C79" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="D79" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E79" s="25" t="s">
-        <v>180</v>
-      </c>
-      <c r="F79" s="19"/>
-      <c r="G79" s="19"/>
-      <c r="H79" s="19"/>
-      <c r="I79" s="19"/>
-      <c r="J79" s="19"/>
-      <c r="K79" s="19"/>
-      <c r="L79" s="22"/>
-      <c r="M79" s="22"/>
-      <c r="N79" s="19"/>
-      <c r="P79" s="23"/>
-      <c r="Q79" s="23"/>
-      <c r="U79" s="23"/>
-    </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="B80" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="C80" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="D80" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E80" s="24" t="s">
-        <v>183</v>
-      </c>
-      <c r="F80" s="19"/>
-      <c r="G80" s="19"/>
-      <c r="H80" s="19"/>
-      <c r="I80" s="19"/>
-      <c r="J80" s="19"/>
-      <c r="K80" s="22"/>
-      <c r="L80" s="22"/>
-      <c r="M80" s="22"/>
-      <c r="N80" s="19"/>
-      <c r="P80" s="23"/>
-      <c r="Q80" s="23"/>
-      <c r="U80" s="23"/>
-    </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="B81" s="20" t="s">
-        <v>184</v>
-      </c>
-      <c r="C81" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="D81" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E81" s="24" t="s">
-        <v>183</v>
-      </c>
-      <c r="F81" s="19"/>
-      <c r="G81" s="19"/>
-      <c r="H81" s="19"/>
-      <c r="I81" s="19"/>
-      <c r="J81" s="19"/>
-      <c r="K81" s="22"/>
-      <c r="L81" s="22"/>
-      <c r="M81" s="22"/>
-      <c r="N81" s="19"/>
-      <c r="P81" s="23"/>
-      <c r="Q81" s="23"/>
-      <c r="U81" s="23"/>
-    </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="26" t="s">
-        <v>161</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="D82" s="6"/>
-      <c r="E82" s="6"/>
-      <c r="F82" s="27"/>
-      <c r="G82" s="28"/>
-      <c r="H82" s="28"/>
-      <c r="I82" s="28"/>
-      <c r="J82" s="28"/>
-      <c r="K82" s="28"/>
-      <c r="L82" s="28"/>
-      <c r="M82" s="28"/>
-      <c r="N82" s="28"/>
-    </row>
-    <row r="83" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="B83" s="20" t="s">
-        <v>188</v>
-      </c>
-      <c r="C83" s="20" t="s">
-        <v>189</v>
-      </c>
-      <c r="D83" s="20"/>
-      <c r="E83" s="24"/>
-      <c r="F83" s="19"/>
-      <c r="G83" s="19"/>
-      <c r="H83" s="19"/>
-      <c r="I83" s="19"/>
-      <c r="J83" s="19"/>
-      <c r="K83" s="22"/>
-      <c r="L83" s="22"/>
-      <c r="M83" s="22"/>
-      <c r="N83" s="19"/>
-      <c r="P83" s="23"/>
-      <c r="Q83" s="23"/>
-      <c r="U83" s="23"/>
-    </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="D84" s="6"/>
-      <c r="E84" s="6"/>
-      <c r="F84" s="6"/>
-      <c r="G84" s="6"/>
-      <c r="H84" s="6"/>
-      <c r="I84" s="6"/>
-      <c r="J84" s="6"/>
-      <c r="K84" s="6"/>
-      <c r="L84" s="6"/>
-      <c r="M84" s="6"/>
-      <c r="N84" s="6"/>
-    </row>
-    <row r="85" s="25" customFormat="true" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B85" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="C85" s="20"/>
-      <c r="D85" s="19"/>
-      <c r="E85" s="21"/>
-      <c r="F85" s="19"/>
-      <c r="G85" s="19"/>
-      <c r="H85" s="19"/>
-      <c r="I85" s="22"/>
-      <c r="J85" s="19"/>
-      <c r="K85" s="19"/>
-      <c r="L85" s="22"/>
-      <c r="M85" s="22"/>
-      <c r="N85" s="19"/>
-      <c r="P85" s="23"/>
-      <c r="Q85" s="23"/>
-      <c r="U85" s="23"/>
-    </row>
-    <row r="86" s="18" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="B87" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="C87" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="D87" s="27"/>
-      <c r="E87" s="27"/>
-      <c r="F87" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="G87" s="27"/>
-      <c r="H87" s="27"/>
-      <c r="I87" s="27"/>
-      <c r="J87" s="27"/>
-      <c r="K87" s="27"/>
-      <c r="L87" s="27"/>
-      <c r="M87" s="27"/>
-      <c r="N87" s="27"/>
-    </row>
-    <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="B88" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="C88" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D88" s="28"/>
-      <c r="E88" s="31"/>
-      <c r="F88" s="31"/>
-      <c r="G88" s="31"/>
-      <c r="H88" s="31"/>
-      <c r="I88" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="J88" s="31"/>
-      <c r="K88" s="31"/>
-      <c r="L88" s="31"/>
-      <c r="M88" s="31"/>
-      <c r="N88" s="31"/>
-    </row>
-    <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A89" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="B89" s="27"/>
-      <c r="C89" s="27"/>
-      <c r="D89" s="27"/>
-      <c r="E89" s="27"/>
-      <c r="F89" s="27"/>
-      <c r="G89" s="27"/>
-      <c r="H89" s="27"/>
-      <c r="I89" s="27"/>
-      <c r="J89" s="27"/>
-      <c r="K89" s="27"/>
-      <c r="L89" s="27"/>
-      <c r="M89" s="27"/>
-      <c r="N89" s="27"/>
+      <c r="J74" s="7"/>
+      <c r="K74" s="7"/>
+      <c r="L74" s="7"/>
+      <c r="M74" s="7"/>
+      <c r="N74" s="7"/>
+      <c r="O74" s="8"/>
+      <c r="P74" s="8"/>
+      <c r="Q74" s="8"/>
+      <c r="R74" s="8"/>
+      <c r="S74" s="8"/>
+      <c r="T74" s="8"/>
+      <c r="U74" s="8"/>
+      <c r="V74" s="8"/>
+      <c r="W74" s="8"/>
+      <c r="X74" s="8"/>
+      <c r="Y74" s="8"/>
+      <c r="Z74" s="8"/>
+      <c r="AA74" s="8"/>
+      <c r="AB74" s="8"/>
+      <c r="AC74" s="8"/>
+      <c r="AD74" s="8"/>
+      <c r="AE74" s="8"/>
+      <c r="AF74" s="8"/>
+      <c r="AG74" s="8"/>
+      <c r="AH74" s="8"/>
+      <c r="AI74" s="8"/>
+      <c r="AJ74" s="8"/>
+      <c r="AK74" s="8"/>
+      <c r="AL74" s="8"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A82">
+  <conditionalFormatting sqref="A66">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E82">
+  <conditionalFormatting sqref="E66">
     <cfRule type="containsText" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E82">
+  <conditionalFormatting sqref="E66">
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>AND($A82="begin group", NOT($B82 = ""))</formula>
+      <formula>AND($A66="begin group", NOT($B66 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E82">
+  <conditionalFormatting sqref="E66">
     <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
-      <formula>AND($A82="end group", $B82 = "", $C82 = "", $D82 = "", $E82 = "", $F82 = "", $G82 = "", $H82 = "", $I82 = "", $J82 = "", $K82 = "", $L82 = "", $M82 = "")</formula>
+      <formula>AND($A66="end group", $B66 = "", $C66 = "", $D66 = "", $E66 = "", $F66 = "", $G66 = "", $H66 = "", $I66 = "", $J66 = "", $K66 = "", $L66 = "", $M66 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E82">
+  <conditionalFormatting sqref="E66">
     <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E82">
+  <conditionalFormatting sqref="E66">
     <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
-      <formula>AND($A82="begin repeat", NOT($B82 = ""))</formula>
+      <formula>AND($A66="begin repeat", NOT($B66 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E82">
+  <conditionalFormatting sqref="E66">
     <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
-      <formula>AND($A82="end repeat", $B82 = "", $C82 = "", $D82 = "", $E82 = "", $F82 = "", $G82 = "", $H82 = "", $I82 = "", $J82 = "", $K82 = "", $L82 = "", $M82 = "")</formula>
+      <formula>AND($A66="end repeat", $B66 = "", $C66 = "", $D66 = "", $E66 = "", $F66 = "", $G66 = "", $H66 = "", $I66 = "", $J66 = "", $K66 = "", $L66 = "", $M66 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E84">
+  <conditionalFormatting sqref="E68">
     <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
-      <formula>AND($A84="begin group", NOT($B84 = ""))</formula>
+      <formula>AND($A68="begin group", NOT($B68 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E84">
+  <conditionalFormatting sqref="E68">
     <cfRule type="cellIs" priority="10" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I84">
+  <conditionalFormatting sqref="I68">
     <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
-      <formula>AND($I84 = "", $A84 = "calculate")</formula>
+      <formula>AND($I68 = "", $A68 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C84">
+  <conditionalFormatting sqref="C68">
     <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
-      <formula>AND(AND(NOT($A84 = "end group"), NOT($A84 = "end repeat"), NOT($A84 = "")), $C84 = "")</formula>
+      <formula>AND(AND(NOT($A68 = "end group"), NOT($A68 = "end repeat"), NOT($A68 = "")), $C68 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B84">
+  <conditionalFormatting sqref="B68">
     <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
-      <formula>AND(AND(NOT($A84 = "end group"), NOT($A84 = "end repeat"), NOT($A84 = "")), $B84 = "")</formula>
+      <formula>AND(AND(NOT($A68 = "end group"), NOT($A68 = "end repeat"), NOT($A68 = "")), $B68 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A84">
+  <conditionalFormatting sqref="A68">
     <cfRule type="cellIs" priority="14" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H84">
+  <conditionalFormatting sqref="H68">
     <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
-      <formula>AND(NOT($G84 = ""), $H84 = "")</formula>
+      <formula>AND(NOT($G68 = ""), $H68 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E84">
+  <conditionalFormatting sqref="E68">
     <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
-      <formula>AND($A84="begin repeat", NOT($B84 = ""))</formula>
+      <formula>AND($A68="begin repeat", NOT($B68 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E84">
+  <conditionalFormatting sqref="E68">
     <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
-      <formula>AND($E84 = "", $A84 = "calculate")</formula>
+      <formula>AND($E68 = "", $A68 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E84">
+  <conditionalFormatting sqref="E68">
     <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
-      <formula>AND($A84="end repeat", $B84 = "", $C84 = "", $D84 = "", $E84 = "", $F84 = "", $G84 = "", $H84 = "", $E84 = "", $J84 = "", $K84 = "", $L84 = "", $M84 = "")</formula>
+      <formula>AND($A68="end repeat", $B68 = "", $C68 = "", $D68 = "", $E68 = "", $F68 = "", $G68 = "", $H68 = "", $E68 = "", $J68 = "", $K68 = "", $L68 = "", $M68 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E84">
+  <conditionalFormatting sqref="E68">
     <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
-      <formula>AND($A84="end group", $B84 = "", $C84 = "", $D84 = "", $E84 = "", $F84 = "", $G84 = "", $H84 = "", $E84 = "", $J84 = "", $K84 = "", $L84 = "", $M84 = "")</formula>
+      <formula>AND($A68="end group", $B68 = "", $C68 = "", $D68 = "", $E68 = "", $F68 = "", $G68 = "", $H68 = "", $E68 = "", $J68 = "", $K68 = "", $L68 = "", $M68 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E84">
+  <conditionalFormatting sqref="E68">
     <cfRule type="containsText" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:Y13">
@@ -5287,7 +4501,7 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
     <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27">
-      <formula>COUNTIF($B$2:$B$1052,B13)&gt;1</formula>
+      <formula>COUNTIF($B$2:$B$1036,B13)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:Y13">
@@ -5304,11 +4518,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D11:D13 D82 D84" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D11:D13 D66 D68" type="list">
       <formula1>"yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D3:D7 D87:D89" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D3:D7 D71:D73" type="list">
       <formula1>"yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5336,71 +4550,71 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="37.2297872340426"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="11.331914893617"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="31.0765957446808"/>
-    <col collapsed="false" hidden="false" max="26" min="4" style="0" width="11.331914893617"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="12.2340425531915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="37.9787234042553"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="11.4851063829787"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="31.6765957446808"/>
+    <col collapsed="false" hidden="false" max="26" min="4" style="0" width="11.4851063829787"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="12.4595744680851"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="33" t="s">
-        <v>196</v>
+        <v>166</v>
       </c>
       <c r="B1" s="33" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>197</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="34" t="s">
-        <v>198</v>
+        <v>168</v>
       </c>
       <c r="B2" s="34" t="s">
         <v>44</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="34" t="s">
-        <v>198</v>
+        <v>168</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>200</v>
+        <v>170</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>201</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="20" t="s">
-        <v>202</v>
+        <v>172</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>203</v>
+        <v>173</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>204</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="20" t="s">
-        <v>202</v>
+        <v>172</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>205</v>
+        <v>175</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>206</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="20" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="B6" s="20" t="n">
         <v>1</v>
@@ -5411,7 +4625,7 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="20" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="B7" s="20" t="n">
         <v>2</v>
@@ -5422,7 +4636,7 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="20" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="B8" s="20" t="n">
         <v>3</v>
@@ -5433,7 +4647,7 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="20" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="B9" s="20" t="n">
         <v>4</v>
@@ -5444,7 +4658,7 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="20" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="B10" s="20" t="n">
         <v>5</v>
@@ -5455,7 +4669,7 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="20" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="B11" s="20" t="n">
         <v>6</v>
@@ -5466,7 +4680,7 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="20" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="B12" s="20" t="n">
         <v>7</v>
@@ -5477,7 +4691,7 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="20" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="B13" s="20" t="n">
         <v>8</v>
@@ -5488,7 +4702,7 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="20" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="B14" s="20" t="n">
         <v>9</v>
@@ -5499,7 +4713,7 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="20" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="B15" s="20" t="n">
         <v>10</v>
@@ -5510,7 +4724,7 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="20" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="B16" s="20" t="n">
         <v>11</v>
@@ -5521,7 +4735,7 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="20" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="B17" s="20" t="n">
         <v>12</v>
@@ -5532,7 +4746,7 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="20" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="B18" s="20" t="n">
         <v>13</v>
@@ -5543,7 +4757,7 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="20" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="B19" s="20" t="n">
         <v>14</v>
@@ -5554,288 +4768,288 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="20" t="s">
-        <v>208</v>
+        <v>178</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>209</v>
+        <v>179</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>210</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="20" t="s">
-        <v>208</v>
+        <v>178</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>108</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="20" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>213</v>
+        <v>183</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="20" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>214</v>
+        <v>184</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>215</v>
+        <v>185</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="20" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>216</v>
+        <v>186</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>217</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="20" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>101</v>
+        <v>188</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>102</v>
+        <v>189</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="20" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>218</v>
+        <v>190</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>219</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="20" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>221</v>
-      </c>
-      <c r="C27" s="35" t="s">
-        <v>222</v>
+        <v>193</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="20" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>223</v>
+        <v>195</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>224</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="20" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>225</v>
-      </c>
-      <c r="C29" s="36" t="s">
-        <v>226</v>
+        <v>197</v>
+      </c>
+      <c r="C29" s="35" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="20" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>227</v>
+        <v>199</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>228</v>
+        <v>200</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="20" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>229</v>
+        <v>201</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>230</v>
+        <v>202</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="20" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>231</v>
+        <v>203</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>232</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="20" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>218</v>
+        <v>190</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>219</v>
+        <v>191</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="20" t="s">
-        <v>233</v>
+        <v>205</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>234</v>
+        <v>206</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>235</v>
+        <v>207</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="20" t="s">
-        <v>233</v>
+        <v>205</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>236</v>
+        <v>208</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>237</v>
+        <v>209</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="20" t="s">
-        <v>233</v>
+        <v>205</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="20" t="s">
-        <v>233</v>
+        <v>205</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>101</v>
+        <v>188</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>102</v>
+        <v>189</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="20" t="s">
-        <v>240</v>
+        <v>212</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>241</v>
+        <v>213</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>222</v>
+        <v>194</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="20" t="s">
-        <v>240</v>
+        <v>212</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>242</v>
+        <v>214</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>224</v>
+        <v>196</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="20" t="s">
-        <v>240</v>
+        <v>212</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>214</v>
+        <v>184</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="20" t="s">
-        <v>240</v>
+        <v>212</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>245</v>
+        <v>217</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="20" t="s">
-        <v>240</v>
+        <v>212</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>246</v>
+        <v>218</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>228</v>
+        <v>200</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="20" t="s">
-        <v>240</v>
+        <v>212</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>247</v>
+        <v>219</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>230</v>
+        <v>202</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="20" t="s">
-        <v>240</v>
+        <v>212</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>231</v>
+        <v>203</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>232</v>
+        <v>204</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="20" t="s">
-        <v>240</v>
+        <v>212</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>218</v>
+        <v>190</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>219</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -5862,89 +5076,89 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1446808510638"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3702127659574"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.4553191489362"/>
-    <col collapsed="false" hidden="false" max="26" min="4" style="0" width="11.331914893617"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="12.2340425531915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.6723404255319"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.8936170212766"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.2808510638298"/>
+    <col collapsed="false" hidden="false" max="26" min="4" style="0" width="11.4851063829787"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="12.4595744680851"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="37" t="s">
-        <v>248</v>
-      </c>
-      <c r="B1" s="37" t="s">
-        <v>249</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>250</v>
-      </c>
-      <c r="D1" s="37" t="s">
-        <v>251</v>
-      </c>
-      <c r="E1" s="37" t="s">
-        <v>252</v>
-      </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
-      <c r="S1" s="38"/>
-      <c r="T1" s="38"/>
-      <c r="U1" s="38"/>
-      <c r="V1" s="38"/>
-      <c r="W1" s="38"/>
-      <c r="X1" s="38"/>
-      <c r="Y1" s="38"/>
-      <c r="Z1" s="38"/>
+      <c r="A1" s="36" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>224</v>
+      </c>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
     </row>
     <row r="2" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="39" t="s">
-        <v>253</v>
-      </c>
-      <c r="B2" s="39" t="s">
-        <v>254</v>
+      <c r="A2" s="38" t="s">
+        <v>225</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>226</v>
       </c>
       <c r="C2" s="1" t="str">
         <f aca="true">TEXT(NOW(), "yyyy-mm-dd")</f>
-        <v>2020-08-25</v>
-      </c>
-      <c r="D2" s="39" t="s">
-        <v>255</v>
-      </c>
-      <c r="E2" s="39" t="s">
-        <v>256</v>
-      </c>
-      <c r="F2" s="39"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="40"/>
-      <c r="U2" s="40"/>
-      <c r="V2" s="40"/>
-      <c r="W2" s="40"/>
-      <c r="X2" s="40"/>
-      <c r="Y2" s="40"/>
-      <c r="Z2" s="40"/>
+        <v>2020-08-26</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>227</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="F2" s="38"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="39"/>
+      <c r="W2" s="39"/>
+      <c r="X2" s="39"/>
+      <c r="Y2" s="39"/>
+      <c r="Z2" s="39"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>